<commit_message>
Update benchmark: 2025-09-14 12:35:11 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,7 +626,11 @@
           <t>28,57 TL - 28,57 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr"/>
+      <c r="G2" s="14" t="inlineStr">
+        <is>
+          <t>9 TL - 9 TL</t>
+        </is>
+      </c>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -659,35 +663,35 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
-      <c r="D3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
-        </is>
-      </c>
-      <c r="H3" s="14" t="inlineStr"/>
-      <c r="I3" s="14" t="inlineStr">
+      <c r="G3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -695,35 +699,35 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
-      <c r="D4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
-        </is>
-      </c>
-      <c r="H4" s="14" t="inlineStr"/>
-      <c r="I4" s="14" t="inlineStr">
+      <c r="G4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -731,35 +735,35 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
-      <c r="D5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
-        </is>
-      </c>
-      <c r="H5" s="14" t="inlineStr"/>
-      <c r="I5" s="14" t="inlineStr">
+      <c r="G5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -767,35 +771,35 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
-        <is>
-          <t>4.300,01 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="H6" s="14" t="inlineStr"/>
-      <c r="I6" s="14" t="inlineStr">
+      <c r="G6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -815,7 +819,11 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr"/>
+      <c r="G7" s="14" t="inlineStr">
+        <is>
+          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
+        </is>
+      </c>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -844,35 +852,35 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr"/>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -880,35 +888,35 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr"/>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -916,35 +924,35 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr"/>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -952,35 +960,35 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
-      <c r="D11" s="14" t="inlineStr">
+      <c r="C11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
-        </is>
-      </c>
-      <c r="H11" s="14" t="inlineStr"/>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="G11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
+      <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -993,23 +1001,23 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1017,12 +1025,12 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1030,18 +1038,22 @@
       </c>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
-      <c r="I13" s="14" t="inlineStr">
+      <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1049,31 +1061,35 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
       <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>4.300 TL - 6,09 TL</t>
-        </is>
-      </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="G14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1447,7 +1463,11 @@
           <t>SENET TAHSİLE ALMA</t>
         </is>
       </c>
-      <c r="C24" s="14" t="inlineStr"/>
+      <c r="C24" s="14" t="inlineStr">
+        <is>
+          <t>457,14 TL</t>
+        </is>
+      </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
           <t>476,2 TL</t>
@@ -1495,7 +1515,11 @@
           <t>MUAMELESİZ SENET İADESİ</t>
         </is>
       </c>
-      <c r="C25" s="14" t="inlineStr"/>
+      <c r="C25" s="14" t="inlineStr">
+        <is>
+          <t>380,95 TL</t>
+        </is>
+      </c>
       <c r="D25" s="14" t="inlineStr">
         <is>
           <t>428,58 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-14 13:24:13 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,20 +668,36 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -704,20 +720,36 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -740,20 +772,36 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
+        </is>
+      </c>
       <c r="H5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -776,20 +824,32 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>4.300,01 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="H6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -857,20 +917,36 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
+        </is>
+      </c>
       <c r="H8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -893,20 +969,36 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
+        </is>
+      </c>
       <c r="H9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -929,20 +1021,36 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+        </is>
+      </c>
       <c r="H10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -965,20 +1073,32 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+        </is>
+      </c>
       <c r="H11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1006,10 +1126,18 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -1030,20 +1158,32 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1066,14 +1206,26 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>4.300 TL - 6,09 TL</t>
+        </is>
+      </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>2.100 TL - 4.300 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-16 06:37:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-17 06:37:25 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -698,11 +694,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J3" s="14" t="inlineStr"/>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +712,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -750,11 +738,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J4" s="14" t="inlineStr"/>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +756,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -802,11 +782,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J5" s="14" t="inlineStr"/>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +800,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -850,11 +822,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="J6" s="14" t="inlineStr"/>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,41 +885,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J8" s="14" t="inlineStr"/>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,41 +929,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J9" s="14" t="inlineStr"/>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,41 +973,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J10" s="14" t="inlineStr"/>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1017,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1099,11 +1039,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="J11" s="14" t="inlineStr"/>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1062,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1158,14 +1090,10 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1184,14 +1112,10 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
+      <c r="J13" s="14" t="inlineStr"/>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1206,11 +1130,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1232,11 +1152,7 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.188 TL - 593 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-18 06:38:56 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -694,7 +698,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr"/>
+      <c r="J3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -712,7 +720,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -738,7 +750,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr"/>
+      <c r="J4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -756,7 +772,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,7 +802,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr"/>
+      <c r="J5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -800,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -822,7 +850,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -885,7 +917,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -911,7 +947,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -929,7 +969,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -955,7 +999,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -973,7 +1021,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -999,7 +1051,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1017,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1039,7 +1099,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr"/>
+      <c r="J11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -1062,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1090,7 +1158,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1112,7 +1184,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1130,7 +1206,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1152,7 +1232,11 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.188 TL - 593 TL</t>
+        </is>
+      </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-22 06:39:17 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1160,7 +1160,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-24 06:38:33 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-25 06:42:16 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -698,11 +694,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J3" s="14" t="inlineStr"/>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +712,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -750,11 +738,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J4" s="14" t="inlineStr"/>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +756,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -802,11 +782,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J5" s="14" t="inlineStr"/>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +800,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -850,11 +822,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="J6" s="14" t="inlineStr"/>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,41 +885,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J8" s="14" t="inlineStr"/>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,41 +929,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J9" s="14" t="inlineStr"/>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,41 +973,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J10" s="14" t="inlineStr"/>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1017,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1099,11 +1039,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="J11" s="14" t="inlineStr"/>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1062,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1158,14 +1090,10 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1184,11 +1112,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
+      <c r="J13" s="14" t="inlineStr"/>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1206,11 +1130,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1232,11 +1152,7 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.188 TL - 593 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-09-26 06:38:08 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -694,7 +698,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr"/>
+      <c r="J3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -712,7 +720,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -738,7 +750,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr"/>
+      <c r="J4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -756,7 +772,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,7 +802,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr"/>
+      <c r="J5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -800,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -822,7 +850,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -885,7 +917,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -911,7 +947,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -929,7 +969,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -955,7 +999,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -973,7 +1021,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -999,7 +1051,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1017,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1039,7 +1099,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr"/>
+      <c r="J11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -1062,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1090,7 +1158,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1112,7 +1184,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1130,7 +1206,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1152,7 +1232,11 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.188 TL - 593 TL</t>
+        </is>
+      </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-01 06:38:31 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>Diğer: 700 TL–4.000 TL</t>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-10-03 06:35:53 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -688,11 +688,7 @@
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -740,11 +736,7 @@
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -792,11 +784,7 @@
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -840,11 +828,7 @@
           <t>4.300,01 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -937,11 +921,7 @@
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -989,11 +969,7 @@
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1041,11 +1017,7 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1089,11 +1061,7 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1160,7 +1128,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1174,16 +1142,12 @@
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
+      <c r="H13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1191,7 +1155,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1226,11 +1190,7 @@
           <t>4.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-04 06:34:07 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -688,7 +688,11 @@
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -736,7 +740,11 @@
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -784,7 +792,11 @@
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -828,7 +840,11 @@
           <t>4.300,01 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -921,7 +937,11 @@
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,7 +989,11 @@
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1017,7 +1041,11 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1061,7 +1089,11 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1128,12 +1160,12 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1142,7 +1174,11 @@
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1190,7 +1226,11 @@
           <t>4.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-05 06:37:16 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-06 06:38:20 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+          <t>Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-07 06:38:57 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>Diğer: 700 TL–4.000 TL</t>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-08 06:39:51 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,11 +621,7 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr">
-        <is>
-          <t>28,57 TL - 28,57 TL</t>
-        </is>
-      </c>
+      <c r="F2" s="14" t="inlineStr"/>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -874,11 +870,7 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>%3</t>
-        </is>
-      </c>
+      <c r="F7" s="14" t="inlineStr"/>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-09 06:37:30 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,7 +621,11 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr"/>
+      <c r="F2" s="14" t="inlineStr">
+        <is>
+          <t>28,57 TL - 28,57 TL</t>
+        </is>
+      </c>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -632,11 +636,7 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr">
-        <is>
-          <t>18 TL - 18 TL</t>
-        </is>
-      </c>
+      <c r="I2" s="14" t="inlineStr"/>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -664,11 +664,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -689,11 +685,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -716,11 +708,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -741,11 +729,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -768,11 +752,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -793,11 +773,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -820,11 +796,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -841,11 +813,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -870,7 +838,11 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr"/>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>%3</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -909,21 +881,17 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -934,11 +902,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -961,21 +925,17 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -986,11 +946,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1013,21 +969,17 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1038,11 +990,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1065,11 +1013,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1086,11 +1030,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1118,11 +1058,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1150,11 +1086,7 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1171,11 +1103,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1198,11 +1126,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-10 06:38:28 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -636,7 +636,11 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr"/>
+      <c r="I2" s="14" t="inlineStr">
+        <is>
+          <t>18 TL - 18 TL</t>
+        </is>
+      </c>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -664,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -685,7 +693,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -708,7 +720,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -729,7 +745,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -752,7 +772,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -773,7 +797,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -796,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -813,7 +845,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -881,7 +917,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -902,7 +942,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -925,7 +969,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -946,7 +994,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -969,7 +1021,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -990,7 +1046,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1013,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1030,7 +1094,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1058,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1086,10 +1158,14 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1103,7 +1179,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1111,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1206,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-11 06:34:42 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +716,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +764,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +812,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,11 +901,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,11 +949,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,11 +997,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1045,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1094,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1158,14 +1122,10 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1151,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1206,11 +1166,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-12 06:34:20 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -716,7 +720,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -764,7 +772,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -812,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -901,7 +917,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -949,7 +969,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -997,7 +1021,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1045,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1094,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1122,10 +1158,14 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1166,7 +1206,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-13 06:41:05 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1160,12 +1160,12 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-10-14 06:39:20 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -730,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -782,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -927,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -979,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -1031,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1165,14 +1141,10 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1191,7 +1163,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1216,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-15 06:39:22 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -726,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -774,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -915,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -963,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -1011,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1144,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1163,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-16 06:39:34 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -683,16 +683,8 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
-        </is>
-      </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -735,16 +727,8 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
-        </is>
-      </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -787,16 +771,8 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
-        </is>
-      </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="G5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -835,16 +811,8 @@
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
-        <is>
-          <t>4.300,01 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="G6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -932,16 +900,8 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="G8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -984,16 +944,8 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="G9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1036,16 +988,8 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="G10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1084,16 +1028,8 @@
         </is>
       </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
-        </is>
-      </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="G11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1133,11 +1069,7 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -1165,7 +1097,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1174,11 +1106,7 @@
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1221,16 +1149,8 @@
           <t>1.952,38 TL - 9.523,81 TL</t>
         </is>
       </c>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>4.300 TL - 6,09 TL</t>
-        </is>
-      </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="G14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-17 06:38:30 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -683,8 +683,16 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G3" s="14" t="inlineStr"/>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -727,8 +735,16 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G4" s="14" t="inlineStr"/>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
+        </is>
+      </c>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -771,8 +787,16 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G5" s="14" t="inlineStr"/>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
+        </is>
+      </c>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -811,8 +835,16 @@
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>4.300,01 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -900,8 +932,16 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr"/>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -944,8 +984,16 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr"/>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -988,8 +1036,16 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr"/>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1028,8 +1084,16 @@
         </is>
       </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+        </is>
+      </c>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1069,7 +1133,11 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -1106,7 +1174,11 @@
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1149,8 +1221,16 @@
           <t>1.952,38 TL - 9.523,81 TL</t>
         </is>
       </c>
-      <c r="G14" s="14" t="inlineStr"/>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>4.300 TL - 6,09 TL</t>
+        </is>
+      </c>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-20 06:39:17 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -673,11 +673,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -725,11 +721,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -777,11 +769,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -829,11 +817,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -922,11 +906,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -974,11 +954,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1026,11 +1002,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1078,11 +1050,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1160,14 +1128,10 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -1211,11 +1175,7 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-21 06:46:11 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,11 +616,7 @@
           <t>23,81 TL - 23,81 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr">
-        <is>
-          <t>20 TL - 20 TL</t>
-        </is>
-      </c>
+      <c r="E2" s="14" t="inlineStr"/>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>28,57 TL - 28,57 TL</t>
@@ -673,7 +669,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -721,7 +721,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -769,7 +773,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -817,7 +825,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -906,7 +918,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -954,7 +970,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1002,7 +1022,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1050,7 +1074,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1123,7 +1151,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1131,7 +1159,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -1175,7 +1207,11 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-22 06:39:48 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,7 +616,11 @@
           <t>23,81 TL - 23,81 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr"/>
+      <c r="E2" s="14" t="inlineStr">
+        <is>
+          <t>20 TL - 20 TL</t>
+        </is>
+      </c>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>28,57 TL - 28,57 TL</t>
@@ -674,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -726,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -778,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -923,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -975,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -1027,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1161,14 +1141,10 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1212,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-23 06:39:36 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -726,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -774,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -915,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -963,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -1011,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1144,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1188,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-24 06:36:27 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,21 +668,13 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -720,21 +712,13 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -772,21 +756,13 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -824,11 +800,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,21 +889,13 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -969,21 +933,13 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -1021,21 +977,13 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1073,11 +1021,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1070,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1158,21 +1098,13 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1191,7 +1123,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1206,21 +1138,13 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-25 06:37:17 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,13 +668,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -712,13 +720,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -756,13 +772,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -800,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -889,13 +917,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -933,13 +969,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -977,13 +1021,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1021,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1070,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1095,16 +1155,24 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1123,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1138,13 +1206,21 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-26 06:37:00 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-27 06:43:03 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1155,12 +1155,12 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-30 06:38:18 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1625,11 +1625,7 @@
           <t>476,2 TL</t>
         </is>
       </c>
-      <c r="E24" s="14" t="inlineStr">
-        <is>
-          <t>600 TL</t>
-        </is>
-      </c>
+      <c r="E24" s="14" t="inlineStr"/>
       <c r="F24" s="14" t="inlineStr">
         <is>
           <t>457,14 TL</t>
@@ -1677,11 +1673,7 @@
           <t>428,58 TL</t>
         </is>
       </c>
-      <c r="E25" s="14" t="inlineStr">
-        <is>
-          <t>600 TL</t>
-        </is>
-      </c>
+      <c r="E25" s="14" t="inlineStr"/>
       <c r="F25" s="14" t="inlineStr">
         <is>
           <t>380,95 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-10-31 06:39:31 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,11 +626,7 @@
           <t>28,57 TL - 28,57 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr">
-        <is>
-          <t>9 TL - 9 TL</t>
-        </is>
-      </c>
+      <c r="G2" s="14" t="inlineStr"/>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -879,11 +875,7 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr">
-        <is>
-          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
-        </is>
-      </c>
+      <c r="G7" s="14" t="inlineStr"/>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -1160,12 +1152,12 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1183,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1617,11 @@
           <t>476,2 TL</t>
         </is>
       </c>
-      <c r="E24" s="14" t="inlineStr"/>
+      <c r="E24" s="14" t="inlineStr">
+        <is>
+          <t>600 TL</t>
+        </is>
+      </c>
       <c r="F24" s="14" t="inlineStr">
         <is>
           <t>457,14 TL</t>
@@ -1673,7 +1669,11 @@
           <t>428,58 TL</t>
         </is>
       </c>
-      <c r="E25" s="14" t="inlineStr"/>
+      <c r="E25" s="14" t="inlineStr">
+        <is>
+          <t>600 TL</t>
+        </is>
+      </c>
       <c r="F25" s="14" t="inlineStr">
         <is>
           <t>380,95 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-01 06:35:04 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,7 +626,11 @@
           <t>28,57 TL - 28,57 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr"/>
+      <c r="G2" s="14" t="inlineStr">
+        <is>
+          <t>9 TL - 9 TL</t>
+        </is>
+      </c>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -875,7 +879,11 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr"/>
+      <c r="G7" s="14" t="inlineStr">
+        <is>
+          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
+        </is>
+      </c>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -1147,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1157,7 +1165,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-02 06:37:40 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,11 +621,7 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr">
-        <is>
-          <t>28,57 TL - 28,57 TL</t>
-        </is>
-      </c>
+      <c r="F2" s="14" t="inlineStr"/>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -874,11 +870,7 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>%3</t>
-        </is>
-      </c>
+      <c r="F7" s="14" t="inlineStr"/>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -1160,12 +1152,12 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1183,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-03 06:40:56 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,7 +621,11 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr"/>
+      <c r="F2" s="14" t="inlineStr">
+        <is>
+          <t>28,57 TL - 28,57 TL</t>
+        </is>
+      </c>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -674,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -726,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -778,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -870,7 +862,11 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr"/>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>%3</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -919,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -971,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -1023,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -1152,19 +1136,15 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1183,7 +1163,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1208,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-04 06:39:22 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,11 +611,7 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr">
-        <is>
-          <t>23,81 TL - 23,81 TL</t>
-        </is>
-      </c>
+      <c r="D2" s="14" t="inlineStr"/>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>20 TL - 20 TL</t>
@@ -636,11 +632,7 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr">
-        <is>
-          <t>18 TL - 18 TL</t>
-        </is>
-      </c>
+      <c r="I2" s="14" t="inlineStr"/>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -668,11 +660,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -684,26 +672,18 @@
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
+      <c r="H3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr">
+      <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -716,11 +696,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -732,26 +708,18 @@
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
+      <c r="H4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr">
+      <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -764,11 +732,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -780,26 +744,18 @@
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
+      <c r="H5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr">
+      <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -812,11 +768,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -828,26 +780,18 @@
           <t>4.300,01 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
+      <c r="H6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
+      <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -856,11 +800,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr">
-        <is>
-          <t>%1,6</t>
-        </is>
-      </c>
+      <c r="D7" s="14" t="inlineStr"/>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -905,11 +845,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -921,26 +857,18 @@
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
+      <c r="H8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -953,11 +881,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,26 +893,18 @@
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
+      <c r="H9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -1001,11 +917,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1017,26 +929,18 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
+      <c r="H10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1049,11 +953,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1065,26 +965,18 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
+      <c r="H11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1102,11 +994,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1117,11 +1005,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1134,38 +1018,26 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
+      <c r="H13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1178,11 +1050,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1194,22 +1062,14 @@
           <t>4.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1598,11 +1458,7 @@
           <t>600 TL</t>
         </is>
       </c>
-      <c r="F24" s="14" t="inlineStr">
-        <is>
-          <t>457,14 TL</t>
-        </is>
-      </c>
+      <c r="F24" s="14" t="inlineStr"/>
       <c r="G24" s="14" t="inlineStr">
         <is>
           <t>160 TL</t>
@@ -1650,11 +1506,7 @@
           <t>600 TL</t>
         </is>
       </c>
-      <c r="F25" s="14" t="inlineStr">
-        <is>
-          <t>380,95 TL</t>
-        </is>
-      </c>
+      <c r="F25" s="14" t="inlineStr"/>
       <c r="G25" s="14" t="inlineStr"/>
       <c r="H25" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-05 06:39:58 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,7 +611,11 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr"/>
+      <c r="D2" s="14" t="inlineStr">
+        <is>
+          <t>23,81 TL - 23,81 TL</t>
+        </is>
+      </c>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>20 TL - 20 TL</t>
@@ -632,7 +636,11 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr"/>
+      <c r="I2" s="14" t="inlineStr">
+        <is>
+          <t>18 TL - 18 TL</t>
+        </is>
+      </c>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -660,19 +668,31 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -683,7 +703,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -696,19 +720,31 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -719,7 +755,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -732,19 +772,31 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -755,7 +807,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -768,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -780,7 +840,11 @@
           <t>4.300,01 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -791,7 +855,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -800,7 +868,11 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr"/>
+      <c r="D7" s="14" t="inlineStr">
+        <is>
+          <t>%1,6</t>
+        </is>
+      </c>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -845,19 +917,31 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -868,7 +952,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -881,19 +969,31 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -904,7 +1004,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -917,19 +1021,31 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -940,7 +1056,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -953,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -965,7 +1089,11 @@
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -976,7 +1104,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -994,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1005,7 +1141,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1015,18 +1155,30 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1037,7 +1189,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1050,26 +1206,42 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>4.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1458,7 +1630,11 @@
           <t>600 TL</t>
         </is>
       </c>
-      <c r="F24" s="14" t="inlineStr"/>
+      <c r="F24" s="14" t="inlineStr">
+        <is>
+          <t>457,14 TL</t>
+        </is>
+      </c>
       <c r="G24" s="14" t="inlineStr">
         <is>
           <t>160 TL</t>
@@ -1506,7 +1682,11 @@
           <t>600 TL</t>
         </is>
       </c>
-      <c r="F25" s="14" t="inlineStr"/>
+      <c r="F25" s="14" t="inlineStr">
+        <is>
+          <t>380,95 TL</t>
+        </is>
+      </c>
       <c r="G25" s="14" t="inlineStr"/>
       <c r="H25" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-06 06:40:27 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-07 06:38:56 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -633,7 +633,7 @@
       </c>
       <c r="H2" s="14" t="inlineStr">
         <is>
-          <t>9 TL - 9 TL</t>
+          <t>15 TL - 15 TL</t>
         </is>
       </c>
       <c r="I2" s="14" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
-          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
       <c r="H3" s="14" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
-          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
       <c r="H4" s="14" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
-          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
       <c r="H5" s="14" t="inlineStr">
@@ -837,7 +837,7 @@
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
-          <t>4.300,01 TL - 76,17 TL</t>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
       <c r="H6" s="14" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
       <c r="H8" s="14" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
-          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
       <c r="H9" s="14" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
       <c r="H10" s="14" t="inlineStr">
@@ -1086,7 +1086,7 @@
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
       <c r="H11" s="14" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
-          <t>4.300 TL - 6,09 TL</t>
+          <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
       <c r="H14" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-08 06:37:34 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +716,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +764,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +812,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,11 +901,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,11 +949,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,11 +997,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1045,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1094,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1155,17 +1119,13 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1206,11 +1166,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-09 06:36:57 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -716,7 +720,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -764,7 +772,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -812,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -901,7 +917,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -949,7 +969,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -997,7 +1021,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1045,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1094,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1122,7 +1158,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
@@ -1166,7 +1206,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-10 06:40:41 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -927,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -979,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1031,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1160,19 +1136,15 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1191,7 +1163,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1216,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-11 06:39:58 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -726,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -774,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -915,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -963,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1011,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1141,10 +1165,14 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1163,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-12 06:39:51 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -636,11 +636,7 @@
           <t>15 TL - 15 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr">
-        <is>
-          <t>18 TL - 18 TL</t>
-        </is>
-      </c>
+      <c r="I2" s="14" t="inlineStr"/>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -668,16 +664,8 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -698,11 +686,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J3" s="14" t="inlineStr"/>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,16 +704,8 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -750,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J4" s="14" t="inlineStr"/>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,16 +744,8 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -802,11 +766,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="J5" s="14" t="inlineStr"/>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,16 +784,8 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -850,11 +802,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="J6" s="14" t="inlineStr"/>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,41 +865,29 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J8" s="14" t="inlineStr"/>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,41 +905,29 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J9" s="14" t="inlineStr"/>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,41 +945,29 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="J10" s="14" t="inlineStr"/>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,16 +985,8 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1099,11 +1003,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="J11" s="14" t="inlineStr"/>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1026,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1155,19 +1051,11 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -1184,14 +1072,10 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
+      <c r="J13" s="14" t="inlineStr"/>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1206,16 +1090,8 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>
@@ -1232,11 +1108,7 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.188 TL - 593 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>
@@ -1615,11 +1487,7 @@
           <t>SENET TAHSİLE ALMA</t>
         </is>
       </c>
-      <c r="C24" s="14" t="inlineStr">
-        <is>
-          <t>457,14 TL</t>
-        </is>
-      </c>
+      <c r="C24" s="14" t="inlineStr"/>
       <c r="D24" s="14" t="inlineStr">
         <is>
           <t>476,2 TL</t>
@@ -1667,11 +1535,7 @@
           <t>MUAMELESİZ SENET İADESİ</t>
         </is>
       </c>
-      <c r="C25" s="14" t="inlineStr">
-        <is>
-          <t>380,95 TL</t>
-        </is>
-      </c>
+      <c r="C25" s="14" t="inlineStr"/>
       <c r="D25" s="14" t="inlineStr">
         <is>
           <t>428,58 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-13 06:40:01 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -636,7 +636,11 @@
           <t>15 TL - 15 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr"/>
+      <c r="I2" s="14" t="inlineStr">
+        <is>
+          <t>18 TL - 18 TL</t>
+        </is>
+      </c>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -664,8 +668,16 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
-      <c r="E3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -686,7 +698,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr"/>
+      <c r="J3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -704,8 +720,16 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
-      <c r="E4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -726,7 +750,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr"/>
+      <c r="J4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -744,8 +772,16 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
-      <c r="E5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -766,7 +802,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr"/>
+      <c r="J5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -784,8 +824,16 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -802,7 +850,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -865,8 +917,16 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
-      <c r="E8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="E8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -887,7 +947,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -905,8 +969,16 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
-      <c r="E9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="E9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -927,7 +999,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -945,8 +1021,16 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
-      <c r="E10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="E10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -967,7 +1051,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -985,8 +1073,16 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1003,7 +1099,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr"/>
+      <c r="J11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -1026,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1054,8 +1158,16 @@
           <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
-      <c r="E13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -1072,7 +1184,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1090,8 +1206,16 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
-      <c r="E14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>
@@ -1108,7 +1232,11 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.188 TL - 593 TL</t>
+        </is>
+      </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>
@@ -1487,7 +1615,11 @@
           <t>SENET TAHSİLE ALMA</t>
         </is>
       </c>
-      <c r="C24" s="14" t="inlineStr"/>
+      <c r="C24" s="14" t="inlineStr">
+        <is>
+          <t>457,14 TL</t>
+        </is>
+      </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
           <t>476,2 TL</t>
@@ -1535,7 +1667,11 @@
           <t>MUAMELESİZ SENET İADESİ</t>
         </is>
       </c>
-      <c r="C25" s="14" t="inlineStr"/>
+      <c r="C25" s="14" t="inlineStr">
+        <is>
+          <t>380,95 TL</t>
+        </is>
+      </c>
       <c r="D25" s="14" t="inlineStr">
         <is>
           <t>428,58 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-14 06:39:00 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +716,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +764,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +812,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,11 +901,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,11 +949,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,11 +997,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1045,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1094,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1155,17 +1119,13 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1206,11 +1166,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-16 06:36:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,11 +703,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -716,7 +716,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -747,11 +751,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -764,7 +764,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -795,11 +799,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -812,7 +812,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -839,11 +843,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -901,7 +901,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -932,11 +936,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -949,7 +949,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -980,11 +984,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -997,7 +997,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1028,11 +1032,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1045,7 +1045,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1072,11 +1076,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1094,7 +1094,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1105,11 +1109,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1122,7 +1122,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1149,11 +1153,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1166,7 +1166,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1193,11 +1197,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-17 06:39:51 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -703,7 +699,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -726,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -751,7 +747,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -774,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -799,7 +795,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -843,7 +843,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -911,32 +915,32 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
+      <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
+      <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -959,32 +963,32 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
+      <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
+      <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -1007,32 +1011,32 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
+      <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
+      <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1076,7 +1080,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1109,7 +1117,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1119,12 +1131,12 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1132,11 +1144,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1153,7 +1161,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1176,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1197,7 +1205,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-18 06:37:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -673,22 +673,14 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -721,22 +713,14 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -769,22 +753,14 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -817,22 +793,14 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -910,22 +878,14 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -958,22 +918,14 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1006,22 +958,14 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1054,22 +998,14 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1136,21 +1072,13 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1183,22 +1111,14 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-19 06:38:42 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -673,14 +673,22 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -713,14 +721,22 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -753,14 +769,22 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -793,14 +817,22 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -878,14 +910,22 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -918,14 +958,22 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -958,14 +1006,22 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -998,14 +1054,22 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1067,18 +1131,26 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1091,7 +1163,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1111,14 +1183,22 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
       <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-20 06:38:08 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -716,11 +712,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -764,11 +756,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -812,11 +800,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -905,11 +889,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -953,11 +933,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1001,11 +977,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1049,11 +1021,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1102,11 +1070,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1134,14 +1098,10 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr"/>
@@ -1163,7 +1123,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1178,11 +1138,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-21 06:39:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,13 +668,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -712,13 +720,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -756,13 +772,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -800,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -889,13 +917,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -933,13 +969,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -977,13 +1021,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1021,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1070,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1095,16 +1155,24 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1138,13 +1206,21 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-22 06:34:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,11 +611,7 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr">
-        <is>
-          <t>23,81 TL - 23,81 TL</t>
-        </is>
-      </c>
+      <c r="D2" s="14" t="inlineStr"/>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>20 TL - 20 TL</t>
@@ -636,16 +632,8 @@
           <t>15 TL - 15 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr">
-        <is>
-          <t>18 TL - 18 TL</t>
-        </is>
-      </c>
-      <c r="J2" s="14" t="inlineStr">
-        <is>
-          <t>15 TL - 15 TL</t>
-        </is>
-      </c>
+      <c r="I2" s="14" t="inlineStr"/>
+      <c r="J2" s="14" t="inlineStr"/>
       <c r="K2" s="14" t="inlineStr">
         <is>
           <t>26,25 TL - 26,25 TL</t>
@@ -663,51 +651,23 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
+      <c r="F3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="I3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="J3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr"/>
+      <c r="J3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -715,51 +675,23 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
+      <c r="F4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="I4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr"/>
+      <c r="J4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -767,51 +699,23 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
+      <c r="F5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="I5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="J5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr"/>
+      <c r="J5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -819,16 +723,8 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -840,26 +736,10 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -868,11 +748,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr">
-        <is>
-          <t>%1,6</t>
-        </is>
-      </c>
+      <c r="D7" s="14" t="inlineStr"/>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -890,11 +766,7 @@
         </is>
       </c>
       <c r="I7" s="14" t="inlineStr"/>
-      <c r="J7" s="14" t="inlineStr">
-        <is>
-          <t>%2,5</t>
-        </is>
-      </c>
+      <c r="J7" s="14" t="inlineStr"/>
       <c r="K7" s="14" t="inlineStr">
         <is>
           <t>%3,1</t>
@@ -912,51 +784,23 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="C8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -964,51 +808,23 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="C9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="H9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -1016,51 +832,23 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="C10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="H10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1068,16 +856,8 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1089,26 +869,10 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="H11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr"/>
+      <c r="J11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1121,16 +885,8 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1141,11 +897,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1153,47 +905,19 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1201,47 +925,23 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.188 TL - 593 TL</t>
-        </is>
-      </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1296,7 +996,7 @@
       </c>
       <c r="K15" s="14" t="inlineStr">
         <is>
-          <t>%0,3 Asgari Tutar: 197,72 TL Azami Tutar: 197,72 TL / 249,13 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1364,7 +1064,7 @@
       </c>
       <c r="K17" s="14" t="inlineStr">
         <is>
-          <t>%0,9 Asgari Tutar: 197,72 TL Azami Tutar: 197,72 TL / 2.528,89 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1442,11 +1142,7 @@
           <t>100 TL</t>
         </is>
       </c>
-      <c r="K20" s="14" t="inlineStr">
-        <is>
-          <t>122,59 TL</t>
-        </is>
-      </c>
+      <c r="K20" s="14" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="B21" s="13" t="inlineStr">
@@ -1496,7 +1192,7 @@
       </c>
       <c r="K21" s="14" t="inlineStr">
         <is>
-          <t>%0,9 Asgari Tutar: 371,72 TL Azami Tutar: 371,72 TL / 2.022,72 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1548,7 +1244,7 @@
       </c>
       <c r="K22" s="14" t="inlineStr">
         <is>
-          <t>%0,3 Asgari Tutar: 61,3 TL Azami Tutar: 61,3 TL / 7.596,55 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1598,11 +1294,7 @@
           <t>50 TL</t>
         </is>
       </c>
-      <c r="K23" s="14" t="inlineStr">
-        <is>
-          <t>54 TL</t>
-        </is>
-      </c>
+      <c r="K23" s="14" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
@@ -1655,11 +1347,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr">
-        <is>
-          <t>371,72 TL</t>
-        </is>
-      </c>
+      <c r="K24" s="14" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1703,11 +1391,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr">
-        <is>
-          <t>312 TL</t>
-        </is>
-      </c>
+      <c r="K25" s="14" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-23 06:38:00 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,7 +611,11 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr"/>
+      <c r="D2" s="14" t="inlineStr">
+        <is>
+          <t>23,81 TL - 23,81 TL</t>
+        </is>
+      </c>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>20 TL - 20 TL</t>
@@ -632,8 +636,16 @@
           <t>15 TL - 15 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr"/>
-      <c r="J2" s="14" t="inlineStr"/>
+      <c r="I2" s="14" t="inlineStr">
+        <is>
+          <t>18 TL - 18 TL</t>
+        </is>
+      </c>
+      <c r="J2" s="14" t="inlineStr">
+        <is>
+          <t>15 TL - 15 TL</t>
+        </is>
+      </c>
       <c r="K2" s="14" t="inlineStr">
         <is>
           <t>26,25 TL - 26,25 TL</t>
@@ -651,23 +663,31 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
-      <c r="D3" s="14" t="inlineStr"/>
-      <c r="E3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr">
+      <c r="G3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
-      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr"/>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -675,23 +695,31 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
-      <c r="D4" s="14" t="inlineStr"/>
-      <c r="E4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr">
+      <c r="G4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
-      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr"/>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -699,23 +727,31 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
-      <c r="D5" s="14" t="inlineStr"/>
-      <c r="E5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr">
+      <c r="G5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
-      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr"/>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -723,23 +759,31 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr"/>
-      <c r="E6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
+      <c r="G6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
-      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr"/>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -748,7 +792,11 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr"/>
+      <c r="D7" s="14" t="inlineStr">
+        <is>
+          <t>%1,6</t>
+        </is>
+      </c>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -766,7 +814,11 @@
         </is>
       </c>
       <c r="I7" s="14" t="inlineStr"/>
-      <c r="J7" s="14" t="inlineStr"/>
+      <c r="J7" s="14" t="inlineStr">
+        <is>
+          <t>%2,5</t>
+        </is>
+      </c>
       <c r="K7" s="14" t="inlineStr">
         <is>
           <t>%3,1</t>
@@ -784,23 +836,31 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
-      <c r="D8" s="14" t="inlineStr"/>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="G8" s="14" t="inlineStr"/>
       <c r="H8" s="14" t="inlineStr"/>
-      <c r="I8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J8" s="14" t="inlineStr"/>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -808,23 +868,31 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
-      <c r="D9" s="14" t="inlineStr"/>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="G9" s="14" t="inlineStr"/>
       <c r="H9" s="14" t="inlineStr"/>
-      <c r="I9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J9" s="14" t="inlineStr"/>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -832,23 +900,31 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
-      <c r="D10" s="14" t="inlineStr"/>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="G10" s="14" t="inlineStr"/>
       <c r="H10" s="14" t="inlineStr"/>
-      <c r="I10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J10" s="14" t="inlineStr"/>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -856,23 +932,31 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
-      <c r="D11" s="14" t="inlineStr"/>
-      <c r="E11" s="14" t="inlineStr">
+      <c r="C11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
+      <c r="G11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
-      <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr"/>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -885,19 +969,27 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -905,19 +997,31 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
-      <c r="D13" s="14" t="inlineStr"/>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr"/>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr"/>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -925,23 +1029,27 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
-      <c r="D14" s="14" t="inlineStr"/>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>6.300 TL - 6,09 TL</t>
-        </is>
-      </c>
+      <c r="G14" s="14" t="inlineStr"/>
       <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr"/>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -996,7 +1104,7 @@
       </c>
       <c r="K15" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,3 Asgari Tutar: 197,72 TL Azami Tutar: 197,72 TL / 249,13 TL</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1172,7 @@
       </c>
       <c r="K17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,9 Asgari Tutar: 197,72 TL Azami Tutar: 197,72 TL / 2.528,89 TL</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1250,11 @@
           <t>100 TL</t>
         </is>
       </c>
-      <c r="K20" s="14" t="inlineStr"/>
+      <c r="K20" s="14" t="inlineStr">
+        <is>
+          <t>122,59 TL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="13" t="inlineStr">
@@ -1192,7 +1304,7 @@
       </c>
       <c r="K21" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,9 Asgari Tutar: 371,72 TL Azami Tutar: 371,72 TL / 2.022,72 TL</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1356,7 @@
       </c>
       <c r="K22" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,3 Asgari Tutar: 61,3 TL Azami Tutar: 61,3 TL / 7.596,55 TL</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1406,11 @@
           <t>50 TL</t>
         </is>
       </c>
-      <c r="K23" s="14" t="inlineStr"/>
+      <c r="K23" s="14" t="inlineStr">
+        <is>
+          <t>54 TL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
@@ -1347,7 +1463,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr"/>
+      <c r="K24" s="14" t="inlineStr">
+        <is>
+          <t>371,72 TL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1391,7 +1511,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr"/>
+      <c r="K25" s="14" t="inlineStr">
+        <is>
+          <t>312 TL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-24 06:39:26 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,21 +668,33 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="E3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr"/>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr"/>
+      <c r="J3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -700,21 +712,33 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="E4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr"/>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr"/>
+      <c r="J4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -732,21 +756,33 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="E5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr"/>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="J5" s="14" t="inlineStr"/>
+      <c r="J5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="K5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -764,21 +800,33 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="D6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -841,21 +889,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr"/>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -873,21 +933,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr"/>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -905,21 +977,33 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr"/>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="J10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="K10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -937,21 +1021,33 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
+      <c r="D11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr"/>
+      <c r="J11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="K11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,09 TL - 76,17 TL</t>
@@ -974,14 +1070,14 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -999,24 +1095,32 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1034,17 +1138,29 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
-      <c r="E14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
       <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr"/>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>6.300 TL - 6,09 TL</t>
+        </is>
+      </c>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.188 TL - 593 TL</t>
+        </is>
+      </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>914,14 TL - 4.265,98 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-25 06:40:46 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -631,11 +631,7 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="H2" s="14" t="inlineStr">
-        <is>
-          <t>15 TL - 15 TL</t>
-        </is>
-      </c>
+      <c r="H2" s="14" t="inlineStr"/>
       <c r="I2" s="14" t="inlineStr">
         <is>
           <t>18 TL - 18 TL</t>
@@ -668,13 +664,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -712,13 +716,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -756,13 +768,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -800,7 +820,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -856,11 +880,7 @@
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
         </is>
       </c>
-      <c r="H7" s="14" t="inlineStr">
-        <is>
-          <t>%3,09</t>
-        </is>
-      </c>
+      <c r="H7" s="14" t="inlineStr"/>
       <c r="I7" s="14" t="inlineStr"/>
       <c r="J7" s="14" t="inlineStr">
         <is>
@@ -889,13 +909,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -933,13 +961,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -977,13 +1013,21 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1021,7 +1065,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1070,7 +1118,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1098,13 +1150,21 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1123,7 +1183,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1138,13 +1198,21 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-26 06:40:13 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -613,7 +613,7 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>23,81 TL - 23,81 TL</t>
+          <t>20.623,81 TL - 20.623,81 TL</t>
         </is>
       </c>
       <c r="E2" s="14" t="inlineStr">
@@ -631,7 +631,11 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="H2" s="14" t="inlineStr"/>
+      <c r="H2" s="14" t="inlineStr">
+        <is>
+          <t>15 TL - 15 TL</t>
+        </is>
+      </c>
       <c r="I2" s="14" t="inlineStr">
         <is>
           <t>18 TL - 18 TL</t>
@@ -659,16 +663,8 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -711,16 +707,8 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -763,16 +751,8 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -815,16 +795,8 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -880,7 +852,11 @@
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
         </is>
       </c>
-      <c r="H7" s="14" t="inlineStr"/>
+      <c r="H7" s="14" t="inlineStr">
+        <is>
+          <t>%3,09</t>
+        </is>
+      </c>
       <c r="I7" s="14" t="inlineStr"/>
       <c r="J7" s="14" t="inlineStr">
         <is>
@@ -904,16 +880,8 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -956,16 +924,8 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1008,16 +968,8 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1060,16 +1012,8 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1115,12 +1059,12 @@
       </c>
       <c r="C12" s="14" t="inlineStr">
         <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
+          <t>WU: 0.29 USD–9,51 USD</t>
         </is>
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+          <t>WU: 0,75 USD–; Diğer: 909,5 TL–909,5 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1147,17 +1091,17 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 15.714,29 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 909,5 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1183,7 +1127,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1193,16 +1137,8 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1253,7 +1189,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
+          <t xml:space="preserve">%0,8 Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
       <c r="E15" s="14" t="inlineStr">
@@ -1321,7 +1257,7 @@
       </c>
       <c r="D17" s="14" t="inlineStr">
         <is>
-          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
+          <t xml:space="preserve">%0,8 Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
       <c r="E17" s="14" t="inlineStr">
@@ -1405,7 +1341,7 @@
       </c>
       <c r="D20" s="14" t="inlineStr">
         <is>
-          <t>285,72 TL</t>
+          <t>20.623,81 TL</t>
         </is>
       </c>
       <c r="E20" s="14" t="inlineStr">
@@ -1453,7 +1389,7 @@
       </c>
       <c r="D21" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 428,58 TL Azami Tutar: 428,58 TL / 5.523,81 TL</t>
+          <t xml:space="preserve">%0,5 Asgari Tutar: 20.623,81 TL Azami Tutar: </t>
         </is>
       </c>
       <c r="E21" s="14" t="inlineStr">
@@ -1505,7 +1441,7 @@
       </c>
       <c r="D22" s="14" t="inlineStr">
         <is>
-          <t>%1 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 6.857,15 TL</t>
+          <t xml:space="preserve">%1 Asgari Tutar: 20.623,81 TL Azami Tutar: </t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -1557,7 +1493,7 @@
       </c>
       <c r="D23" s="14" t="inlineStr">
         <is>
-          <t>64,77 TL</t>
+          <t>20.623,81 TL</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -1614,7 +1550,7 @@
       </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
-          <t>476,2 TL</t>
+          <t>20.623,81 TL</t>
         </is>
       </c>
       <c r="E24" s="14" t="inlineStr">
@@ -1666,7 +1602,7 @@
       </c>
       <c r="D25" s="14" t="inlineStr">
         <is>
-          <t>428,58 TL</t>
+          <t>20.623,81 TL</t>
         </is>
       </c>
       <c r="E25" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-28 06:41:25 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -613,7 +613,7 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>20.623,81 TL - 20.623,81 TL</t>
+          <t>23,81 TL - 23,81 TL</t>
         </is>
       </c>
       <c r="E2" s="14" t="inlineStr">
@@ -663,8 +663,16 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -707,8 +715,16 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -751,8 +767,16 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -795,8 +819,16 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -880,8 +912,16 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -924,8 +964,16 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -968,8 +1016,16 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1012,8 +1068,16 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1059,12 +1123,12 @@
       </c>
       <c r="C12" s="14" t="inlineStr">
         <is>
-          <t>WU: 0.29 USD–9,51 USD</t>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>WU: 0,75 USD–; Diğer: 909,5 TL–909,5 TL</t>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1091,12 +1155,12 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 15.714,29 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 909,5 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1137,8 +1201,16 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1189,7 +1261,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">%0,8 Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
         </is>
       </c>
       <c r="E15" s="14" t="inlineStr">
@@ -1257,7 +1329,7 @@
       </c>
       <c r="D17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">%0,8 Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
         </is>
       </c>
       <c r="E17" s="14" t="inlineStr">
@@ -1341,7 +1413,7 @@
       </c>
       <c r="D20" s="14" t="inlineStr">
         <is>
-          <t>20.623,81 TL</t>
+          <t>285,72 TL</t>
         </is>
       </c>
       <c r="E20" s="14" t="inlineStr">
@@ -1389,7 +1461,7 @@
       </c>
       <c r="D21" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">%0,5 Asgari Tutar: 20.623,81 TL Azami Tutar: </t>
+          <t>%0,5 Asgari Tutar: 428,58 TL Azami Tutar: 428,58 TL / 5.523,81 TL</t>
         </is>
       </c>
       <c r="E21" s="14" t="inlineStr">
@@ -1441,7 +1513,7 @@
       </c>
       <c r="D22" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">%1 Asgari Tutar: 20.623,81 TL Azami Tutar: </t>
+          <t>%1 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 6.857,15 TL</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -1493,7 +1565,7 @@
       </c>
       <c r="D23" s="14" t="inlineStr">
         <is>
-          <t>20.623,81 TL</t>
+          <t>64,77 TL</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -1550,7 +1622,7 @@
       </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
-          <t>20.623,81 TL</t>
+          <t>476,2 TL</t>
         </is>
       </c>
       <c r="E24" s="14" t="inlineStr">
@@ -1602,7 +1674,7 @@
       </c>
       <c r="D25" s="14" t="inlineStr">
         <is>
-          <t>20.623,81 TL</t>
+          <t>428,58 TL</t>
         </is>
       </c>
       <c r="E25" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-11-29 06:36:43 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,11 +626,7 @@
           <t>28,57 TL - 28,57 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr">
-        <is>
-          <t>9 TL - 9 TL</t>
-        </is>
-      </c>
+      <c r="G2" s="14" t="inlineStr"/>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -678,11 +674,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,11 +722,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,11 +770,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -879,11 +863,7 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr">
-        <is>
-          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
-        </is>
-      </c>
+      <c r="G7" s="14" t="inlineStr"/>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -927,11 +907,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -979,11 +955,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1031,11 +1003,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1155,7 +1123,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1168,11 +1136,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1216,11 +1180,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-11-30 06:38:50 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,7 +626,11 @@
           <t>28,57 TL - 28,57 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr"/>
+      <c r="G2" s="14" t="inlineStr">
+        <is>
+          <t>9 TL - 9 TL</t>
+        </is>
+      </c>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -674,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -722,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -770,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -863,7 +879,11 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr"/>
+      <c r="G7" s="14" t="inlineStr">
+        <is>
+          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
+        </is>
+      </c>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -907,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -955,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1003,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1123,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1136,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1180,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-01 06:42:14 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +716,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +764,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +812,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,11 +901,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,11 +949,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,11 +997,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1045,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1094,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1158,11 +1122,7 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1206,11 +1166,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1655,11 +1611,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr">
-        <is>
-          <t>371,72 TL</t>
-        </is>
-      </c>
+      <c r="K24" s="14" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1703,11 +1655,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr">
-        <is>
-          <t>312 TL</t>
-        </is>
-      </c>
+      <c r="K25" s="14" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-02 06:41:41 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,12 +663,12 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -711,12 +711,12 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -759,12 +759,12 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -807,12 +807,12 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -896,12 +896,12 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -944,12 +944,12 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -992,12 +992,12 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1040,12 +1040,12 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
+      <c r="C11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1089,12 +1089,12 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1117,12 +1117,12 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1161,12 +1161,12 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1611,7 +1611,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr"/>
+      <c r="K24" s="14" t="inlineStr">
+        <is>
+          <t>371,72 TL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1655,7 +1659,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr"/>
+      <c r="K25" s="14" t="inlineStr">
+        <is>
+          <t>312 TL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-03 06:41:04 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,7 +663,11 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -674,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -711,7 +711,11 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -722,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -759,7 +759,11 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -770,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -807,7 +807,11 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -896,7 +900,11 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -907,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -944,7 +948,11 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -955,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -992,7 +996,11 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1003,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1040,7 +1044,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1089,10 +1097,14 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>Diğer: 700 TL–4.000 TL</t>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1117,10 +1129,14 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1128,11 +1144,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1161,7 +1173,11 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>
@@ -1172,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-04 06:40:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -699,11 +699,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -747,11 +743,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -795,11 +787,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -843,11 +831,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -936,11 +920,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -984,11 +964,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -1032,11 +1008,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1080,11 +1052,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1117,11 +1085,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1136,7 +1100,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1161,11 +1125,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1205,11 +1165,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-05 06:41:12 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,17 +668,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,7 +699,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -712,17 +716,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -743,7 +747,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -756,17 +764,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -787,7 +795,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -800,11 +812,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -831,7 +839,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -889,17 +901,17 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -920,7 +932,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -933,17 +949,17 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -964,7 +980,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -977,17 +997,17 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1008,7 +1028,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1021,11 +1045,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1052,7 +1072,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1070,11 +1094,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1085,7 +1105,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1098,17 +1122,17 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1125,7 +1149,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1138,17 +1166,17 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1165,7 +1193,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-06 06:36:58 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,7 +668,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -716,7 +720,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -764,7 +772,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -812,7 +824,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -901,7 +917,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -949,7 +969,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -997,7 +1021,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1045,7 +1073,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1094,7 +1126,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1122,7 +1158,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
@@ -1151,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1206,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-08 06:44:06 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +716,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +764,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,11 +812,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,11 +901,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -969,11 +949,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1021,11 +997,7 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1073,11 +1045,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1126,11 +1094,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1158,14 +1122,10 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1206,11 +1166,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-09 06:41:45 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,17 +668,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,11 +699,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -716,17 +712,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -747,11 +743,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -764,17 +756,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -795,11 +787,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -812,7 +800,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -839,11 +831,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -901,42 +889,38 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
+      <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -949,42 +933,38 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
+      <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -997,42 +977,38 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
+      <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1045,7 +1021,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1072,11 +1052,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1094,7 +1070,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1105,11 +1085,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1122,17 +1098,17 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1149,11 +1125,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1166,17 +1138,17 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1193,11 +1165,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-10 06:42:04 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,7 +703,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -722,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -743,7 +755,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -766,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -787,7 +807,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -831,7 +855,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -899,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -920,7 +952,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -943,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -964,7 +1004,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -987,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1008,7 +1056,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1052,7 +1104,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1085,7 +1141,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1108,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1125,7 +1189,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1148,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1165,7 +1237,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-11 06:42:51 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -927,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -979,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1031,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1168,11 +1144,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1216,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-12 06:41:48 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -726,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -774,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -915,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -963,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1011,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1144,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1188,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-13 06:38:35 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,11 +726,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,11 +774,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -927,11 +915,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -979,11 +963,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1031,11 +1011,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1168,11 +1144,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1216,11 +1188,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-14 06:39:06 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -726,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -774,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -915,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -963,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1011,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1144,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1188,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-15 06:44:32 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,11 +663,7 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -715,11 +711,7 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -767,11 +759,7 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -819,11 +807,7 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -912,11 +896,7 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -964,11 +944,7 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1016,11 +992,7 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1068,11 +1040,7 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1121,11 +1089,7 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1153,11 +1117,7 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -1201,11 +1161,7 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-16 06:42:40 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,7 +663,11 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -711,7 +715,11 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -759,7 +767,11 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -807,7 +819,11 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -896,7 +912,11 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -944,7 +964,11 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -992,7 +1016,11 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1040,7 +1068,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1089,7 +1121,11 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1117,7 +1153,11 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -1161,7 +1201,11 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-17 06:42:20 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -643,7 +643,7 @@
       </c>
       <c r="J2" s="14" t="inlineStr">
         <is>
-          <t>15 TL - 15 TL</t>
+          <t>25 TL - 25 TL</t>
         </is>
       </c>
       <c r="K2" s="14" t="inlineStr">
@@ -1160,12 +1160,12 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-18 06:42:29 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+          <t>Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-19 06:40:51 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -703,11 +703,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -755,11 +751,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -807,11 +799,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -855,11 +843,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -952,11 +936,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -1004,11 +984,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -1056,11 +1032,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1104,11 +1076,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1128,7 +1096,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>Diğer: 700 TL–4.000 TL</t>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -1141,11 +1109,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1189,11 +1153,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1237,11 +1197,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-20 06:39:26 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -703,7 +703,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -751,7 +755,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -799,7 +807,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -843,7 +855,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -936,7 +952,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -984,7 +1004,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -1032,7 +1056,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1076,7 +1104,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1109,7 +1141,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1119,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1129,7 +1165,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1153,7 +1189,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1197,7 +1237,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-21 06:39:29 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,11 +668,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -683,11 +679,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="inlineStr"/>
       <c r="H3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,11 +712,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -735,11 +723,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="inlineStr"/>
       <c r="H4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,11 +756,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -787,11 +767,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="G5" s="14" t="inlineStr"/>
       <c r="H5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,22 +800,14 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="D6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="G6" s="14" t="inlineStr"/>
       <c r="H6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,26 +885,18 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="G8" s="14" t="inlineStr"/>
       <c r="H8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -969,26 +929,18 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="G9" s="14" t="inlineStr"/>
       <c r="H9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1021,26 +973,18 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="G10" s="14" t="inlineStr"/>
       <c r="H10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1073,22 +1017,14 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
+      <c r="D11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="G11" s="14" t="inlineStr"/>
       <c r="H11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1126,18 +1062,10 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -1155,17 +1083,13 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1191,7 +1115,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1206,11 +1130,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1221,11 +1141,7 @@
           <t>1.952,38 TL - 9.523,81 TL</t>
         </is>
       </c>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>6.300 TL - 6,09 TL</t>
-        </is>
-      </c>
+      <c r="G14" s="14" t="inlineStr"/>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>2.100 TL - 4.300 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-22 06:45:37 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -641,11 +641,7 @@
           <t>18 TL - 18 TL</t>
         </is>
       </c>
-      <c r="J2" s="14" t="inlineStr">
-        <is>
-          <t>25 TL - 25 TL</t>
-        </is>
-      </c>
+      <c r="J2" s="14" t="inlineStr"/>
       <c r="K2" s="14" t="inlineStr">
         <is>
           <t>26,25 TL - 26,25 TL</t>
@@ -668,7 +664,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -679,7 +679,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -712,7 +716,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -723,7 +731,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -756,7 +768,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -767,7 +783,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="G5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="H5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -800,14 +820,22 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="H6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -858,11 +886,7 @@
         </is>
       </c>
       <c r="I7" s="14" t="inlineStr"/>
-      <c r="J7" s="14" t="inlineStr">
-        <is>
-          <t>%2,5</t>
-        </is>
-      </c>
+      <c r="J7" s="14" t="inlineStr"/>
       <c r="K7" s="14" t="inlineStr">
         <is>
           <t>%3,1</t>
@@ -885,7 +909,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -896,7 +924,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
       <c r="H8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -929,7 +961,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -940,7 +976,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
       <c r="H9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -973,7 +1013,11 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -984,7 +1028,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
       <c r="H10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1017,14 +1065,22 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="H11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1062,10 +1118,18 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -1086,10 +1150,14 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1130,7 +1198,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>2.300 TL - 9.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
@@ -1141,7 +1213,11 @@
           <t>1.952,38 TL - 9.523,81 TL</t>
         </is>
       </c>
-      <c r="G14" s="14" t="inlineStr"/>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>6.300 TL - 6,09 TL</t>
+        </is>
+      </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>2.100 TL - 4.300 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-23 06:43:16 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -641,7 +641,11 @@
           <t>18 TL - 18 TL</t>
         </is>
       </c>
-      <c r="J2" s="14" t="inlineStr"/>
+      <c r="J2" s="14" t="inlineStr">
+        <is>
+          <t>25 TL - 25 TL</t>
+        </is>
+      </c>
       <c r="K2" s="14" t="inlineStr">
         <is>
           <t>26,25 TL - 26,25 TL</t>
@@ -669,11 +673,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -721,11 +721,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -773,11 +769,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -825,11 +817,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -886,7 +874,11 @@
         </is>
       </c>
       <c r="I7" s="14" t="inlineStr"/>
-      <c r="J7" s="14" t="inlineStr"/>
+      <c r="J7" s="14" t="inlineStr">
+        <is>
+          <t>%2,5</t>
+        </is>
+      </c>
       <c r="K7" s="14" t="inlineStr">
         <is>
           <t>%3,1</t>
@@ -914,11 +906,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -966,11 +954,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1018,11 +1002,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1070,11 +1050,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1147,19 +1123,15 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -1183,7 +1155,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1203,11 +1175,7 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-24 06:43:58 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1123,7 +1123,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1615,11 +1615,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr">
-        <is>
-          <t>371,72 TL</t>
-        </is>
-      </c>
+      <c r="K24" s="14" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1663,11 +1659,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr">
-        <is>
-          <t>312 TL</t>
-        </is>
-      </c>
+      <c r="K25" s="14" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-25 06:43:11 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,11 +621,7 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr">
-        <is>
-          <t>28,57 TL - 28,57 TL</t>
-        </is>
-      </c>
+      <c r="F2" s="14" t="inlineStr"/>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -673,22 +669,18 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -721,22 +713,18 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -769,22 +757,18 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -817,18 +801,18 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -858,11 +842,7 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>%3</t>
-        </is>
-      </c>
+      <c r="F7" s="14" t="inlineStr"/>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -906,22 +886,18 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -954,22 +930,18 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1002,22 +974,18 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1050,18 +1018,18 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1131,18 +1099,14 @@
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr"/>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1175,22 +1139,18 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr"/>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
@@ -1615,7 +1575,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr"/>
+      <c r="K24" s="14" t="inlineStr">
+        <is>
+          <t>371,72 TL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1659,7 +1623,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr"/>
+      <c r="K25" s="14" t="inlineStr">
+        <is>
+          <t>312 TL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2025-12-26 06:41:35 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,7 +621,11 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr"/>
+      <c r="F2" s="14" t="inlineStr">
+        <is>
+          <t>28,57 TL - 28,57 TL</t>
+        </is>
+      </c>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -674,13 +678,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -718,13 +730,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -762,13 +782,21 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -812,7 +840,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -842,7 +874,11 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr"/>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>%3</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -891,13 +927,21 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -935,13 +979,21 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -979,13 +1031,21 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1029,7 +1089,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1096,7 +1160,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1104,9 +1168,17 @@
           <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1144,13 +1216,21 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-27 06:40:02 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,21 +678,13 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,21 +722,13 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,21 +766,13 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -840,11 +816,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -927,21 +899,13 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -979,21 +943,13 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1031,21 +987,13 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1089,11 +1037,7 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1160,30 +1104,22 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
+      <c r="H13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1191,7 +1127,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1216,21 +1152,13 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
@@ -1261,7 +1189,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
       <c r="E15" s="14" t="inlineStr">
@@ -1329,7 +1257,7 @@
       </c>
       <c r="D17" s="14" t="inlineStr">
         <is>
-          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
       <c r="E17" s="14" t="inlineStr">
@@ -1411,11 +1339,7 @@
           <t>85,71 TL</t>
         </is>
       </c>
-      <c r="D20" s="14" t="inlineStr">
-        <is>
-          <t>285,72 TL</t>
-        </is>
-      </c>
+      <c r="D20" s="14" t="inlineStr"/>
       <c r="E20" s="14" t="inlineStr">
         <is>
           <t>300 TL</t>
@@ -1461,7 +1385,7 @@
       </c>
       <c r="D21" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 428,58 TL Azami Tutar: 428,58 TL / 5.523,81 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
       <c r="E21" s="14" t="inlineStr">
@@ -1513,7 +1437,7 @@
       </c>
       <c r="D22" s="14" t="inlineStr">
         <is>
-          <t>%1 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 6.857,15 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -1563,11 +1487,7 @@
           <t>66,67 TL</t>
         </is>
       </c>
-      <c r="D23" s="14" t="inlineStr">
-        <is>
-          <t>64,77 TL</t>
-        </is>
-      </c>
+      <c r="D23" s="14" t="inlineStr"/>
       <c r="E23" s="14" t="inlineStr">
         <is>
           <t>60 TL</t>
@@ -1620,11 +1540,7 @@
           <t>457,14 TL</t>
         </is>
       </c>
-      <c r="D24" s="14" t="inlineStr">
-        <is>
-          <t>476,2 TL</t>
-        </is>
-      </c>
+      <c r="D24" s="14" t="inlineStr"/>
       <c r="E24" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>
@@ -1672,11 +1588,7 @@
           <t>380,95 TL</t>
         </is>
       </c>
-      <c r="D25" s="14" t="inlineStr">
-        <is>
-          <t>428,58 TL</t>
-        </is>
-      </c>
+      <c r="D25" s="14" t="inlineStr"/>
       <c r="E25" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-28 06:40:41 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -673,18 +673,22 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -717,18 +721,22 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -761,18 +769,22 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -805,18 +817,18 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -894,18 +906,22 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -938,18 +954,22 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="E9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -982,18 +1002,22 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1026,18 +1050,18 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1107,14 +1131,18 @@
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1127,7 +1155,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1147,18 +1175,22 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
@@ -1189,7 +1221,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
         </is>
       </c>
       <c r="E15" s="14" t="inlineStr">
@@ -1257,7 +1289,7 @@
       </c>
       <c r="D17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,8 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 3.047,62 TL</t>
         </is>
       </c>
       <c r="E17" s="14" t="inlineStr">
@@ -1339,7 +1371,11 @@
           <t>85,71 TL</t>
         </is>
       </c>
-      <c r="D20" s="14" t="inlineStr"/>
+      <c r="D20" s="14" t="inlineStr">
+        <is>
+          <t>285,72 TL</t>
+        </is>
+      </c>
       <c r="E20" s="14" t="inlineStr">
         <is>
           <t>300 TL</t>
@@ -1385,7 +1421,7 @@
       </c>
       <c r="D21" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,5 Asgari Tutar: 428,58 TL Azami Tutar: 428,58 TL / 5.523,81 TL</t>
         </is>
       </c>
       <c r="E21" s="14" t="inlineStr">
@@ -1437,7 +1473,7 @@
       </c>
       <c r="D22" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%1 Asgari Tutar: 285,72 TL Azami Tutar: 285,72 TL / 6.857,15 TL</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -1487,7 +1523,11 @@
           <t>66,67 TL</t>
         </is>
       </c>
-      <c r="D23" s="14" t="inlineStr"/>
+      <c r="D23" s="14" t="inlineStr">
+        <is>
+          <t>64,77 TL</t>
+        </is>
+      </c>
       <c r="E23" s="14" t="inlineStr">
         <is>
           <t>60 TL</t>
@@ -1540,7 +1580,11 @@
           <t>457,14 TL</t>
         </is>
       </c>
-      <c r="D24" s="14" t="inlineStr"/>
+      <c r="D24" s="14" t="inlineStr">
+        <is>
+          <t>476,2 TL</t>
+        </is>
+      </c>
       <c r="E24" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>
@@ -1588,7 +1632,11 @@
           <t>380,95 TL</t>
         </is>
       </c>
-      <c r="D25" s="14" t="inlineStr"/>
+      <c r="D25" s="14" t="inlineStr">
+        <is>
+          <t>428,58 TL</t>
+        </is>
+      </c>
       <c r="E25" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-29 06:44:35 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -606,11 +606,7 @@
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr"/>
-      <c r="C2" s="14" t="inlineStr">
-        <is>
-          <t>25 TL - 25 TL</t>
-        </is>
-      </c>
+      <c r="C2" s="14" t="inlineStr"/>
       <c r="D2" s="14" t="inlineStr">
         <is>
           <t>23,81 TL - 23,81 TL</t>
@@ -621,11 +617,7 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr">
-        <is>
-          <t>28,57 TL - 28,57 TL</t>
-        </is>
-      </c>
+      <c r="F2" s="14" t="inlineStr"/>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -673,12 +665,12 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -721,12 +713,12 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -769,12 +761,12 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -817,7 +809,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -858,11 +854,7 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>%3</t>
-        </is>
-      </c>
+      <c r="F7" s="14" t="inlineStr"/>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -906,12 +898,12 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -954,12 +946,12 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1002,12 +994,12 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1050,7 +1042,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1091,7 +1087,7 @@
       </c>
       <c r="C12" s="14" t="inlineStr">
         <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
+          <t>WU: 1.000,01 USD–</t>
         </is>
       </c>
       <c r="D12" s="14" t="inlineStr">
@@ -1123,7 +1119,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1131,12 +1127,12 @@
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr"/>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1155,7 +1151,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>
@@ -1175,12 +1171,12 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr"/>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-30 06:42:47 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -606,7 +606,11 @@
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr"/>
-      <c r="C2" s="14" t="inlineStr"/>
+      <c r="C2" s="14" t="inlineStr">
+        <is>
+          <t>25 TL - 25 TL</t>
+        </is>
+      </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
           <t>23,81 TL - 23,81 TL</t>
@@ -617,7 +621,11 @@
           <t>20 TL - 20 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr"/>
+      <c r="F2" s="14" t="inlineStr">
+        <is>
+          <t>28,57 TL - 28,57 TL</t>
+        </is>
+      </c>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>9 TL - 9 TL</t>
@@ -655,11 +663,7 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -670,7 +674,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -703,11 +711,7 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -718,7 +722,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -751,11 +759,7 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -766,7 +770,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -799,11 +807,7 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -854,7 +858,11 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr"/>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>%3</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -888,11 +896,7 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -903,7 +907,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -936,11 +944,7 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -951,7 +955,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -984,11 +992,7 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -999,7 +1003,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1032,11 +1040,7 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1085,11 +1089,7 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1117,11 +1117,7 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -1129,10 +1125,14 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1161,11 +1161,7 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>
@@ -1176,7 +1172,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2025-12-31 06:43:47 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,11 +611,7 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr">
-        <is>
-          <t>23,81 TL - 23,81 TL</t>
-        </is>
-      </c>
+      <c r="D2" s="14" t="inlineStr"/>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>20 TL - 20 TL</t>
@@ -689,11 +685,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -737,11 +729,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -785,11 +773,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -829,11 +813,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -852,11 +832,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr">
-        <is>
-          <t>%1,6</t>
-        </is>
-      </c>
+      <c r="D7" s="14" t="inlineStr"/>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -922,11 +898,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -970,11 +942,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1018,11 +986,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1062,11 +1026,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1120,12 +1080,12 @@
       <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1139,11 +1099,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1151,7 +1107,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-01 06:42:35 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -549,7 +549,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>BENCHMARKING-2025</t>
+          <t>BENCHMARKING-2026</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr"/>
@@ -611,7 +611,11 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr"/>
+      <c r="D2" s="14" t="inlineStr">
+        <is>
+          <t>23,81 TL - 23,81 TL</t>
+        </is>
+      </c>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>20 TL - 20 TL</t>
@@ -659,17 +663,17 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -685,17 +689,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -703,17 +707,17 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -729,17 +733,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -747,17 +751,17 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -773,17 +777,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -791,17 +795,17 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -813,17 +817,17 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -832,7 +836,11 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr"/>
+      <c r="D7" s="14" t="inlineStr">
+        <is>
+          <t>%1,6</t>
+        </is>
+      </c>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -872,43 +880,43 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H8" s="14" t="inlineStr">
+      <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr"/>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -916,43 +924,43 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="E9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H9" s="14" t="inlineStr">
+      <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr"/>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -960,43 +968,43 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
+      <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr"/>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1004,17 +1012,17 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1026,17 +1034,17 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1049,7 +1057,11 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1065,11 +1077,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1077,17 +1085,17 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -1099,17 +1107,17 @@
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1117,17 +1125,17 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>
@@ -1149,11 +1157,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1502,7 +1506,7 @@
       </c>
       <c r="I23" s="14" t="inlineStr">
         <is>
-          <t>80 TL</t>
+          <t>350 TL</t>
         </is>
       </c>
       <c r="J23" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-02 06:43:00 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -673,12 +673,12 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,7 +699,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -717,12 +721,12 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -743,7 +747,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -761,12 +769,12 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -787,7 +795,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -805,7 +817,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -827,7 +843,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -890,12 +910,12 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -916,7 +936,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -934,12 +958,12 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -960,7 +984,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -978,12 +1006,12 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1004,7 +1032,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1022,7 +1054,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1044,7 +1080,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1077,7 +1117,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1087,20 +1131,20 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr"/>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1117,7 +1161,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1135,12 +1183,12 @@
           <t>2.300 TL - 9.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr"/>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1157,7 +1205,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-03 06:39:58 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -608,7 +608,7 @@
       <c r="B2" s="13" t="inlineStr"/>
       <c r="C2" s="14" t="inlineStr">
         <is>
-          <t>25 TL - 25 TL</t>
+          <t>30 TL - 30 TL</t>
         </is>
       </c>
       <c r="D2" s="14" t="inlineStr">
@@ -678,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -726,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -774,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -915,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -963,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1011,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1131,7 +1155,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1144,7 +1168,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1188,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-04 06:40:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -693,11 +689,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,11 +722,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -745,11 +733,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,11 +766,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -797,11 +777,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -845,11 +821,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -927,11 +899,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -942,11 +910,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -979,11 +943,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -994,11 +954,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1031,11 +987,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1046,11 +998,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1094,11 +1042,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1165,25 +1109,17 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1191,7 +1127,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 53,19 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1216,11 +1152,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-05 06:47:52 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,28 +678,28 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G3" s="14" t="inlineStr"/>
       <c r="H3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -722,28 +722,28 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="inlineStr"/>
       <c r="H4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -766,28 +766,28 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G5" s="14" t="inlineStr"/>
       <c r="H5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -811,27 +811,23 @@
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
+      <c r="G6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
+      <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -899,28 +895,28 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G8" s="14" t="inlineStr"/>
       <c r="H8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -943,28 +939,28 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G9" s="14" t="inlineStr"/>
       <c r="H9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -987,28 +983,28 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G10" s="14" t="inlineStr"/>
       <c r="H10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1032,27 +1028,23 @@
         </is>
       </c>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
+      <c r="G11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
+      <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
+      <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr"/>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1077,19 +1069,11 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1099,7 +1083,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1109,27 +1093,31 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1152,12 +1140,12 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>6.300 TL - 6,09 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
+      <c r="G14" s="14" t="inlineStr"/>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>2.100 TL - 4.300 TL</t>
@@ -1169,11 +1157,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>914,14 TL - 4.265,98 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-06 06:43:47 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -678,11 +678,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr"/>
       <c r="H3" s="14" t="inlineStr">
         <is>
@@ -699,7 +695,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr"/>
+      <c r="K3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -722,11 +722,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr"/>
       <c r="H4" s="14" t="inlineStr">
         <is>
@@ -743,7 +739,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr"/>
+      <c r="K4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -766,11 +766,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr"/>
       <c r="H5" s="14" t="inlineStr">
         <is>
@@ -787,7 +783,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr"/>
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -827,7 +827,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -895,11 +899,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr"/>
       <c r="H8" s="14" t="inlineStr">
         <is>
@@ -916,7 +916,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K8" s="14" t="inlineStr"/>
+      <c r="K8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -939,11 +943,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr"/>
       <c r="H9" s="14" t="inlineStr">
         <is>
@@ -960,7 +960,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K9" s="14" t="inlineStr"/>
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -983,11 +987,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr"/>
       <c r="H10" s="14" t="inlineStr">
         <is>
@@ -1004,7 +1004,11 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="K10" s="14" t="inlineStr"/>
+      <c r="K10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -1044,7 +1048,11 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr"/>
+      <c r="K11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1073,7 +1081,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1088,19 +1100,15 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1117,7 +1125,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1140,11 +1152,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr"/>
       <c r="H14" s="14" t="inlineStr">
         <is>
@@ -1157,7 +1165,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>914,14 TL - 4.265,98 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1536,11 +1548,7 @@
           <t>457,14 TL</t>
         </is>
       </c>
-      <c r="D24" s="14" t="inlineStr">
-        <is>
-          <t>476,2 TL</t>
-        </is>
-      </c>
+      <c r="D24" s="14" t="inlineStr"/>
       <c r="E24" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>
@@ -1566,11 +1574,7 @@
           <t>20 TL</t>
         </is>
       </c>
-      <c r="J24" s="14" t="inlineStr">
-        <is>
-          <t>375 TL</t>
-        </is>
-      </c>
+      <c r="J24" s="14" t="inlineStr"/>
       <c r="K24" s="14" t="inlineStr">
         <is>
           <t>371,72 TL</t>
@@ -1588,11 +1592,7 @@
           <t>380,95 TL</t>
         </is>
       </c>
-      <c r="D25" s="14" t="inlineStr">
-        <is>
-          <t>428,58 TL</t>
-        </is>
-      </c>
+      <c r="D25" s="14" t="inlineStr"/>
       <c r="E25" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>
@@ -1614,11 +1614,7 @@
           <t>230 TL</t>
         </is>
       </c>
-      <c r="J25" s="14" t="inlineStr">
-        <is>
-          <t>375 TL</t>
-        </is>
-      </c>
+      <c r="J25" s="14" t="inlineStr"/>
       <c r="K25" s="14" t="inlineStr">
         <is>
           <t>312 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-07 06:43:19 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,11 +663,7 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -678,13 +674,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr"/>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -707,11 +707,7 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -722,13 +718,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr"/>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -751,11 +751,7 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -766,13 +762,17 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr"/>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
+      <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -795,28 +795,24 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
+      <c r="F6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -884,11 +880,7 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -899,13 +891,17 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr"/>
-      <c r="H8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -928,11 +924,7 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -943,13 +935,17 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr"/>
-      <c r="H9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -972,11 +968,7 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -987,13 +979,17 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr"/>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1016,28 +1012,24 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
+      <c r="C11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
+      <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
+      <c r="F11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1065,11 +1057,7 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1077,7 +1065,11 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -1093,11 +1085,7 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
@@ -1105,16 +1093,16 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 851,5 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1137,11 +1125,7 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>
@@ -1152,13 +1136,17 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr"/>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>2.100 TL - 4.300 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>6.300 TL - 6,09 TL</t>
+        </is>
+      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
@@ -1548,7 +1536,11 @@
           <t>457,14 TL</t>
         </is>
       </c>
-      <c r="D24" s="14" t="inlineStr"/>
+      <c r="D24" s="14" t="inlineStr">
+        <is>
+          <t>476,2 TL</t>
+        </is>
+      </c>
       <c r="E24" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>
@@ -1574,7 +1566,11 @@
           <t>20 TL</t>
         </is>
       </c>
-      <c r="J24" s="14" t="inlineStr"/>
+      <c r="J24" s="14" t="inlineStr">
+        <is>
+          <t>375 TL</t>
+        </is>
+      </c>
       <c r="K24" s="14" t="inlineStr">
         <is>
           <t>371,72 TL</t>
@@ -1592,7 +1588,11 @@
           <t>380,95 TL</t>
         </is>
       </c>
-      <c r="D25" s="14" t="inlineStr"/>
+      <c r="D25" s="14" t="inlineStr">
+        <is>
+          <t>428,58 TL</t>
+        </is>
+      </c>
       <c r="E25" s="14" t="inlineStr">
         <is>
           <t>600 TL</t>
@@ -1614,7 +1614,11 @@
           <t>230 TL</t>
         </is>
       </c>
-      <c r="J25" s="14" t="inlineStr"/>
+      <c r="J25" s="14" t="inlineStr">
+        <is>
+          <t>375 TL</t>
+        </is>
+      </c>
       <c r="K25" s="14" t="inlineStr">
         <is>
           <t>312 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-08 06:43:43 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,7 +663,11 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -684,7 +688,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr"/>
+      <c r="H3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -707,7 +715,11 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -728,7 +740,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr"/>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -751,7 +767,11 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,7 +792,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr"/>
+      <c r="H5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -795,7 +819,11 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -812,7 +840,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -880,7 +912,11 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -901,7 +937,11 @@
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr"/>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -924,7 +964,11 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -945,7 +989,11 @@
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr"/>
+      <c r="H9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -968,7 +1016,11 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -989,7 +1041,11 @@
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr"/>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
+        </is>
+      </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -1012,7 +1068,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1029,7 +1089,11 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr"/>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
+        </is>
+      </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1057,7 +1121,11 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1085,15 +1153,19 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1102,7 +1174,11 @@
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
@@ -1125,7 +1201,11 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>2.300 TL - 9.500 TL</t>
@@ -1146,7 +1226,11 @@
           <t>6.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>2.100 TL - 4.300 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-09 06:43:26 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,11 +616,7 @@
           <t>23,81 TL - 23,81 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr">
-        <is>
-          <t>20 TL - 20 TL</t>
-        </is>
-      </c>
+      <c r="E2" s="14" t="inlineStr"/>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>28,57 TL - 28,57 TL</t>
@@ -648,7 +644,7 @@
       </c>
       <c r="K2" s="14" t="inlineStr">
         <is>
-          <t>26,25 TL - 26,25 TL</t>
+          <t>32,62 TL - 32,62 TL</t>
         </is>
       </c>
     </row>
@@ -678,11 +674,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -730,11 +722,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -782,11 +770,7 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -927,11 +911,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -979,11 +959,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1031,11 +1007,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1155,12 +1127,12 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr">
@@ -1168,11 +1140,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1216,11 +1184,7 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1296,7 +1260,7 @@
       </c>
       <c r="K15" s="14" t="inlineStr">
         <is>
-          <t>%0,3 Asgari Tutar: 197,72 TL Azami Tutar: 197,72 TL / 249,13 TL</t>
+          <t>%0,3 Asgari Tutar: 237,26 TL Azami Tutar: 237,26 TL / 298,96 TL</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1328,7 @@
       </c>
       <c r="K17" s="14" t="inlineStr">
         <is>
-          <t>%0,9 Asgari Tutar: 197,72 TL Azami Tutar: 197,72 TL / 2.528,89 TL</t>
+          <t>%0,6 Asgari Tutar: 237,26 TL Azami Tutar: 237,26 TL / 3.034,67 TL</t>
         </is>
       </c>
     </row>
@@ -1444,7 +1408,7 @@
       </c>
       <c r="K20" s="14" t="inlineStr">
         <is>
-          <t>122,59 TL</t>
+          <t>147,11 TL</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1460,7 @@
       </c>
       <c r="K21" s="14" t="inlineStr">
         <is>
-          <t>%0,9 Asgari Tutar: 371,72 TL Azami Tutar: 371,72 TL / 2.022,72 TL</t>
+          <t>%0,9 Asgari Tutar: 446,06 TL Azami Tutar: 446,06 TL / 2.427,26 TL</t>
         </is>
       </c>
     </row>
@@ -1548,7 +1512,7 @@
       </c>
       <c r="K22" s="14" t="inlineStr">
         <is>
-          <t>%0,3 Asgari Tutar: 61,3 TL Azami Tutar: 61,3 TL / 7.596,55 TL</t>
+          <t>%0,3 Asgari Tutar: 73,56 TL Azami Tutar: 73,56 TL / 9.115,86 TL</t>
         </is>
       </c>
     </row>
@@ -1600,7 +1564,7 @@
       </c>
       <c r="K23" s="14" t="inlineStr">
         <is>
-          <t>54 TL</t>
+          <t>64,8 TL</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1621,7 @@
       </c>
       <c r="K24" s="14" t="inlineStr">
         <is>
-          <t>371,72 TL</t>
+          <t>446,06 TL</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1669,7 @@
       </c>
       <c r="K25" s="14" t="inlineStr">
         <is>
-          <t>312 TL</t>
+          <t>374,4 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-13 06:43:33 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,7 +616,11 @@
           <t>23,81 TL - 23,81 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr"/>
+      <c r="E2" s="14" t="inlineStr">
+        <is>
+          <t>20 TL - 20 TL</t>
+        </is>
+      </c>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>28,57 TL - 28,57 TL</t>
@@ -674,7 +678,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -722,7 +730,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -770,7 +782,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -911,7 +927,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -959,7 +979,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1007,7 +1031,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1137,10 +1165,14 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1184,7 +1216,11 @@
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-15 06:43:29 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -668,36 +668,20 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
+      <c r="D3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
+      <c r="H3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="I3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -720,36 +704,20 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
+      <c r="D4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
+      <c r="H4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="I4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -772,36 +740,20 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
+      <c r="D5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
+      <c r="H5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="H5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="I5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -824,16 +776,8 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -845,11 +789,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -917,21 +857,9 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="E8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D8" s="14" t="inlineStr"/>
+      <c r="E8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -942,11 +870,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -969,21 +893,9 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="E9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D9" s="14" t="inlineStr"/>
+      <c r="E9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -994,11 +906,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1021,21 +929,9 @@
           <t>14,29 TL - 28,57 TL - 300 TL</t>
         </is>
       </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="D10" s="14" t="inlineStr"/>
+      <c r="E10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1046,11 +942,7 @@
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
@@ -1073,16 +965,8 @@
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="D11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -1094,11 +978,7 @@
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
@@ -1126,11 +1006,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1155,35 +1031,19 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 300 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
-        </is>
-      </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1206,21 +1066,9 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>2.300 TL - 9.500 TL</t>
-        </is>
-      </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1239,7 +1087,7 @@
       </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
-          <t>914,14 TL - 4.265,98 TL</t>
+          <t>2.000 TL - 24.000 TL</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1144,7 @@
       </c>
       <c r="K15" s="14" t="inlineStr">
         <is>
-          <t>%0,3 Asgari Tutar: 237,26 TL Azami Tutar: 237,26 TL / 298,96 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1364,7 +1212,7 @@
       </c>
       <c r="K17" s="14" t="inlineStr">
         <is>
-          <t>%0,6 Asgari Tutar: 237,26 TL Azami Tutar: 237,26 TL / 3.034,67 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1442,11 +1290,7 @@
           <t>100 TL</t>
         </is>
       </c>
-      <c r="K20" s="14" t="inlineStr">
-        <is>
-          <t>147,11 TL</t>
-        </is>
-      </c>
+      <c r="K20" s="14" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="B21" s="13" t="inlineStr">
@@ -1496,7 +1340,7 @@
       </c>
       <c r="K21" s="14" t="inlineStr">
         <is>
-          <t>%0,9 Asgari Tutar: 446,06 TL Azami Tutar: 446,06 TL / 2.427,26 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1548,7 +1392,7 @@
       </c>
       <c r="K22" s="14" t="inlineStr">
         <is>
-          <t>%0,3 Asgari Tutar: 73,56 TL Azami Tutar: 73,56 TL / 9.115,86 TL</t>
+          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
         </is>
       </c>
     </row>
@@ -1598,11 +1442,7 @@
           <t>50 TL</t>
         </is>
       </c>
-      <c r="K23" s="14" t="inlineStr">
-        <is>
-          <t>64,8 TL</t>
-        </is>
-      </c>
+      <c r="K23" s="14" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
@@ -1655,11 +1495,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr">
-        <is>
-          <t>446,06 TL</t>
-        </is>
-      </c>
+      <c r="K24" s="14" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1703,11 +1539,7 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr">
-        <is>
-          <t>374,4 TL</t>
-        </is>
-      </c>
+      <c r="K25" s="14" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-16 06:43:39 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,35 +663,35 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
-      <c r="E3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H3" s="14" t="inlineStr">
+      <c r="H3" s="14" t="inlineStr"/>
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="B4" s="13" t="inlineStr">
@@ -699,35 +699,35 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
-      <c r="E4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H4" s="14" t="inlineStr">
+      <c r="H4" s="14" t="inlineStr"/>
+      <c r="I4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="B5" s="13" t="inlineStr">
@@ -735,35 +735,35 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
-      <c r="E5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
+      <c r="H5" s="14" t="inlineStr"/>
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="B6" s="13" t="inlineStr">
@@ -771,13 +771,17 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -786,20 +790,20 @@
       </c>
       <c r="H6" s="14" t="inlineStr">
         <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
+      <c r="I6" s="14" t="inlineStr">
+        <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -852,35 +856,35 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D8" s="14" t="inlineStr"/>
-      <c r="E8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr"/>
+      <c r="D8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="E8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H8" s="14" t="inlineStr">
+      <c r="H8" s="14" t="inlineStr"/>
+      <c r="I8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="J8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I8" s="14" t="inlineStr"/>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="B9" s="13" t="inlineStr">
@@ -888,35 +892,35 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D9" s="14" t="inlineStr"/>
-      <c r="E9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr"/>
+      <c r="D9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="E9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H9" s="14" t="inlineStr">
+      <c r="H9" s="14" t="inlineStr"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="J9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I9" s="14" t="inlineStr"/>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="B10" s="13" t="inlineStr">
@@ -924,35 +928,35 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
-      <c r="D10" s="14" t="inlineStr"/>
-      <c r="E10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr"/>
+      <c r="D10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="E10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
+      <c r="H10" s="14" t="inlineStr"/>
+      <c r="I10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
+      <c r="J10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,72 TL</t>
         </is>
       </c>
-      <c r="I10" s="14" t="inlineStr"/>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -960,35 +964,35 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
+      <c r="C11" s="14" t="inlineStr"/>
+      <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr"/>
-      <c r="E11" s="14" t="inlineStr"/>
+      <c r="E11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
+      <c r="H11" s="14" t="inlineStr"/>
+      <c r="I11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="J11" s="14" t="inlineStr">
         <is>
           <t>3,05 TL - 6,1 TL - 76,18 TL</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr"/>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1001,12 +1005,12 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1017,11 +1021,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1029,31 +1029,35 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
-      <c r="E13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+        </is>
+      </c>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
+          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
+        </is>
+      </c>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
           <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1061,13 +1065,13 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr"/>
-      <c r="E14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>1.660 TL - 1.660 TL</t>
+        </is>
+      </c>
       <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
@@ -1076,7 +1080,7 @@
       </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
-          <t>2.100 TL - 4.300 TL</t>
+          <t>3.000 TL - 6.000 TL</t>
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
@@ -1085,11 +1089,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>2.000 TL - 24.000 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="K15" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,3 Asgari Tutar: 237,26 TL Azami Tutar: 237,26 TL / 298,96 TL</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="H17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar: 160 TL Azami Tutar: 160 TL / 160 TL / 160 TL</t>
+          <t xml:space="preserve"> Asgari Tutar: 210 TL Azami Tutar: 210 TL / 210 TL / 210 TL</t>
         </is>
       </c>
       <c r="I17" s="14" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="K17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,6 Asgari Tutar: 237,26 TL Azami Tutar: 237,26 TL / 3.034,67 TL</t>
         </is>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       <c r="G20" s="14" t="inlineStr"/>
       <c r="H20" s="14" t="inlineStr">
         <is>
-          <t>72 TL</t>
+          <t>100 TL</t>
         </is>
       </c>
       <c r="I20" s="14" t="inlineStr">
@@ -1290,7 +1290,11 @@
           <t>100 TL</t>
         </is>
       </c>
-      <c r="K20" s="14" t="inlineStr"/>
+      <c r="K20" s="14" t="inlineStr">
+        <is>
+          <t>147,11 TL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="13" t="inlineStr">
@@ -1325,7 +1329,7 @@
       </c>
       <c r="H21" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 1.950 TL Azami Tutar: 1.950 TL</t>
+          <t>%0,5 Asgari Tutar: 2.750 TL Azami Tutar: 2.750 TL</t>
         </is>
       </c>
       <c r="I21" s="14" t="inlineStr">
@@ -1340,7 +1344,7 @@
       </c>
       <c r="K21" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,9 Asgari Tutar: 446,06 TL Azami Tutar: 446,06 TL / 2.427,26 TL</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1381,7 @@
       </c>
       <c r="H22" s="14" t="inlineStr">
         <is>
-          <t>%0,7 Asgari Tutar: 290 TL Azami Tutar: 290 TL / 290 TL</t>
+          <t>%0,7 Asgari Tutar: 400 TL Azami Tutar: 400 TL / 400 TL</t>
         </is>
       </c>
       <c r="I22" s="14" t="inlineStr">
@@ -1392,7 +1396,7 @@
       </c>
       <c r="K22" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar:  Azami Tutar: </t>
+          <t>%0,3 Asgari Tutar: 73,56 TL Azami Tutar: 73,56 TL / 9.115,86 TL</t>
         </is>
       </c>
     </row>
@@ -1429,7 +1433,7 @@
       </c>
       <c r="H23" s="14" t="inlineStr">
         <is>
-          <t>43,5 TL</t>
+          <t>57,5 TL</t>
         </is>
       </c>
       <c r="I23" s="14" t="inlineStr">
@@ -1442,7 +1446,11 @@
           <t>50 TL</t>
         </is>
       </c>
-      <c r="K23" s="14" t="inlineStr"/>
+      <c r="K23" s="14" t="inlineStr">
+        <is>
+          <t>64,8 TL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
@@ -1482,7 +1490,7 @@
       </c>
       <c r="H24" s="14" t="inlineStr">
         <is>
-          <t>250 TL</t>
+          <t>350 TL</t>
         </is>
       </c>
       <c r="I24" s="14" t="inlineStr">
@@ -1495,7 +1503,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K24" s="14" t="inlineStr"/>
+      <c r="K24" s="14" t="inlineStr">
+        <is>
+          <t>446,06 TL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="13" t="inlineStr">
@@ -1526,7 +1538,7 @@
       <c r="G25" s="14" t="inlineStr"/>
       <c r="H25" s="14" t="inlineStr">
         <is>
-          <t>290 TL</t>
+          <t>400 TL</t>
         </is>
       </c>
       <c r="I25" s="14" t="inlineStr">
@@ -1539,7 +1551,11 @@
           <t>375 TL</t>
         </is>
       </c>
-      <c r="K25" s="14" t="inlineStr"/>
+      <c r="K25" s="14" t="inlineStr">
+        <is>
+          <t>374,4 TL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-17 06:39:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -636,11 +636,7 @@
           <t>15 TL - 15 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr">
-        <is>
-          <t>18 TL - 18 TL</t>
-        </is>
-      </c>
+      <c r="I2" s="14" t="inlineStr"/>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>25 TL - 25 TL</t>
@@ -663,7 +659,11 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -674,7 +674,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,7 +703,11 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -710,7 +718,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -735,7 +747,11 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -746,7 +762,11 @@
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -771,7 +791,11 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -803,7 +827,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -856,7 +884,11 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -867,7 +899,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -892,7 +928,11 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -903,7 +943,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -928,7 +972,11 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -939,7 +987,11 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -964,7 +1016,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1005,7 +1061,11 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1021,7 +1081,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1029,7 +1093,11 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -1040,7 +1108,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1057,7 +1129,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1065,14 +1141,22 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1089,7 +1173,11 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>2.000 TL - 24.000 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-18 06:40:46 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -636,7 +636,11 @@
           <t>15 TL - 15 TL</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr"/>
+      <c r="I2" s="14" t="inlineStr">
+        <is>
+          <t>18 TL - 18 TL</t>
+        </is>
+      </c>
       <c r="J2" s="14" t="inlineStr">
         <is>
           <t>25 TL - 25 TL</t>
@@ -1105,7 +1109,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-19 06:47:45 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,26 +663,18 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr">
+      <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -707,26 +699,18 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr">
+      <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -751,26 +735,18 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr">
+      <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -795,11 +771,7 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -831,11 +803,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -888,11 +856,7 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -903,11 +867,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -932,11 +892,7 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -947,11 +903,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -976,11 +928,7 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -991,11 +939,7 @@
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -1020,11 +964,7 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -1065,11 +1005,7 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -1085,11 +1021,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1097,11 +1029,7 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -1109,14 +1037,10 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 8.700 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1133,11 +1057,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1145,22 +1065,14 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>1.660 TL - 1.660 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>
@@ -1177,11 +1089,7 @@
           <t>1.188 TL - 593 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>2.000 TL - 24.000 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-20 06:45:27 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -646,11 +646,7 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="K2" s="14" t="inlineStr">
-        <is>
-          <t>32,62 TL - 32,62 TL</t>
-        </is>
-      </c>
+      <c r="K2" s="14" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
@@ -663,12 +659,12 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
-      <c r="D3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -681,16 +677,8 @@
         </is>
       </c>
       <c r="H3" s="14" t="inlineStr"/>
-      <c r="I3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="J3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I3" s="14" t="inlineStr"/>
+      <c r="J3" s="14" t="inlineStr"/>
       <c r="K3" s="14" t="inlineStr"/>
     </row>
     <row r="4">
@@ -699,12 +687,12 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
-      <c r="D4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -717,16 +705,8 @@
         </is>
       </c>
       <c r="H4" s="14" t="inlineStr"/>
-      <c r="I4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="inlineStr"/>
+      <c r="J4" s="14" t="inlineStr"/>
       <c r="K4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
@@ -735,12 +715,12 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
-      <c r="D5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
+      <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -753,16 +733,8 @@
         </is>
       </c>
       <c r="H5" s="14" t="inlineStr"/>
-      <c r="I5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="J5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="I5" s="14" t="inlineStr"/>
+      <c r="J5" s="14" t="inlineStr"/>
       <c r="K5" s="14" t="inlineStr"/>
     </row>
     <row r="6">
@@ -771,12 +743,12 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
@@ -795,15 +767,19 @@
       </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+          <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
       <c r="J6" s="14" t="inlineStr">
         <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="K6" s="14" t="inlineStr"/>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -839,11 +815,7 @@
           <t>%2,5</t>
         </is>
       </c>
-      <c r="K7" s="14" t="inlineStr">
-        <is>
-          <t>%3,1</t>
-        </is>
-      </c>
+      <c r="K7" s="14" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="12" t="inlineStr">
@@ -856,12 +828,12 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
-      <c r="D8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -874,16 +846,8 @@
         </is>
       </c>
       <c r="H8" s="14" t="inlineStr"/>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="I8" s="14" t="inlineStr"/>
+      <c r="J8" s="14" t="inlineStr"/>
       <c r="K8" s="14" t="inlineStr"/>
     </row>
     <row r="9">
@@ -892,12 +856,12 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
-      <c r="D9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -910,16 +874,8 @@
         </is>
       </c>
       <c r="H9" s="14" t="inlineStr"/>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="I9" s="14" t="inlineStr"/>
+      <c r="J9" s="14" t="inlineStr"/>
       <c r="K9" s="14" t="inlineStr"/>
     </row>
     <row r="10">
@@ -928,12 +884,12 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
+      <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
@@ -946,16 +902,8 @@
         </is>
       </c>
       <c r="H10" s="14" t="inlineStr"/>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,72 TL</t>
-        </is>
-      </c>
+      <c r="I10" s="14" t="inlineStr"/>
+      <c r="J10" s="14" t="inlineStr"/>
       <c r="K10" s="14" t="inlineStr"/>
     </row>
     <row r="11">
@@ -964,12 +912,12 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
-      <c r="D11" s="14" t="inlineStr">
+      <c r="C11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
         </is>
       </c>
+      <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr">
         <is>
           <t>3,04 TL - 6,09 TL - 76,17 TL</t>
@@ -982,16 +930,8 @@
         </is>
       </c>
       <c r="H11" s="14" t="inlineStr"/>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>3,05 TL - 6,1 TL - 76,18 TL</t>
-        </is>
-      </c>
+      <c r="I11" s="14" t="inlineStr"/>
+      <c r="J11" s="14" t="inlineStr"/>
       <c r="K11" s="14" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1005,12 +945,12 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -1021,7 +961,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 12 USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -1029,12 +973,12 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -1049,7 +993,7 @@
       </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 6,09 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
       <c r="J13" s="14" t="inlineStr">
@@ -1057,7 +1001,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1065,7 +1013,11 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
@@ -1086,10 +1038,14 @@
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
-          <t>1.188 TL - 593 TL</t>
-        </is>
-      </c>
-      <c r="K14" s="14" t="inlineStr"/>
+          <t>1.554,97 TL - 7.784 TL</t>
+        </is>
+      </c>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>2.000 TL - 24.000 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-21 06:46:01 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -646,7 +646,11 @@
           <t>25 TL - 25 TL</t>
         </is>
       </c>
-      <c r="K2" s="14" t="inlineStr"/>
+      <c r="K2" s="14" t="inlineStr">
+        <is>
+          <t>32,62 TL - 32,62 TL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
@@ -659,18 +663,14 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr"/>
+      <c r="D3" s="14" t="inlineStr"/>
+      <c r="E3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D3" s="14" t="inlineStr"/>
-      <c r="E3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -687,18 +687,14 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
+      <c r="C4" s="14" t="inlineStr"/>
+      <c r="D4" s="14" t="inlineStr"/>
+      <c r="E4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D4" s="14" t="inlineStr"/>
-      <c r="E4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -715,18 +711,14 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr"/>
+      <c r="D5" s="14" t="inlineStr"/>
+      <c r="E5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
         </is>
       </c>
-      <c r="D5" s="14" t="inlineStr"/>
-      <c r="E5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
-      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -743,17 +735,13 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="inlineStr"/>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -815,7 +803,11 @@
           <t>%2,5</t>
         </is>
       </c>
-      <c r="K7" s="14" t="inlineStr"/>
+      <c r="K7" s="14" t="inlineStr">
+        <is>
+          <t>%3,1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="12" t="inlineStr">
@@ -828,18 +820,14 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr"/>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -856,18 +844,14 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr"/>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="E9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -884,18 +868,14 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr"/>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 304,71 TL</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -912,17 +892,9 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr"/>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
@@ -945,12 +917,12 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -963,7 +935,7 @@
       <c r="J12" s="14" t="inlineStr"/>
       <c r="K12" s="14" t="inlineStr">
         <is>
-          <t>WU: 12 USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
         </is>
       </c>
     </row>
@@ -973,18 +945,18 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
+      <c r="E13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1003,7 +975,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1013,18 +985,18 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr"/>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>1.660 TL - 1.660 TL</t>
-        </is>
-      </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
+      <c r="E14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-22 06:44:41 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -613,12 +613,12 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>23,81 TL - 23,81 TL</t>
+          <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
       <c r="E2" s="14" t="inlineStr">
         <is>
-          <t>20 TL - 20 TL</t>
+          <t>26 TL - 26 TL</t>
         </is>
       </c>
       <c r="F2" s="14" t="inlineStr">
@@ -631,11 +631,7 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="H2" s="14" t="inlineStr">
-        <is>
-          <t>15 TL - 15 TL</t>
-        </is>
-      </c>
+      <c r="H2" s="14" t="inlineStr"/>
       <c r="I2" s="14" t="inlineStr">
         <is>
           <t>18 TL - 18 TL</t>
@@ -663,7 +659,11 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr">
@@ -687,7 +687,11 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr">
@@ -711,7 +715,11 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr">
@@ -735,13 +743,17 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="D6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -792,11 +804,7 @@
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
         </is>
       </c>
-      <c r="H7" s="14" t="inlineStr">
-        <is>
-          <t>%3,09</t>
-        </is>
-      </c>
+      <c r="H7" s="14" t="inlineStr"/>
       <c r="I7" s="14" t="inlineStr"/>
       <c r="J7" s="14" t="inlineStr">
         <is>
@@ -820,7 +828,11 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr">
@@ -844,7 +856,11 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr">
@@ -868,7 +884,11 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr">
@@ -892,7 +912,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
@@ -917,12 +941,12 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -945,13 +969,17 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+        </is>
+      </c>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
@@ -985,13 +1013,17 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
-      <c r="E14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>2.170 TL - 2.170 TL</t>
+        </is>
+      </c>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>1.952,38 TL - 9.523,81 TL</t>
@@ -1042,7 +1074,7 @@
       </c>
       <c r="E15" s="14" t="inlineStr">
         <is>
-          <t>%0,6 Asgari Tutar: 280 TL Azami Tutar: 280 TL / 12.000 TL</t>
+          <t>%0,6 Asgari Tutar: 350 TL Azami Tutar: 350 TL / 15.000 TL</t>
         </is>
       </c>
       <c r="F15" s="14" t="inlineStr">
@@ -1110,7 +1142,7 @@
       </c>
       <c r="E17" s="14" t="inlineStr">
         <is>
-          <t>%0,6 Asgari Tutar: 300 TL Azami Tutar: 300 TL / 3.250 TL</t>
+          <t>%0,6 Asgari Tutar: 390 TL Azami Tutar: 390 TL / 4.200 TL</t>
         </is>
       </c>
       <c r="F17" s="14" t="inlineStr">
@@ -1194,7 +1226,7 @@
       </c>
       <c r="E20" s="14" t="inlineStr">
         <is>
-          <t>300 TL</t>
+          <t>390 TL</t>
         </is>
       </c>
       <c r="F20" s="14" t="inlineStr">
@@ -1242,7 +1274,7 @@
       </c>
       <c r="E21" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 1.250 TL Azami Tutar: 1.250 TL / 12.500 TL</t>
+          <t>%0,5 Asgari Tutar: 1.630 TL Azami Tutar: 1.630 TL / 16.360 TL</t>
         </is>
       </c>
       <c r="F21" s="14" t="inlineStr">
@@ -1294,7 +1326,7 @@
       </c>
       <c r="E22" s="14" t="inlineStr">
         <is>
-          <t>%1 Asgari Tutar: 900 TL Azami Tutar: 900 TL / 22.500 TL</t>
+          <t>%1 Asgari Tutar: 1.170 TL Azami Tutar: 1.170 TL / 29.450 TL</t>
         </is>
       </c>
       <c r="F22" s="14" t="inlineStr">
@@ -1346,7 +1378,7 @@
       </c>
       <c r="E23" s="14" t="inlineStr">
         <is>
-          <t>60 TL</t>
+          <t>75 TL</t>
         </is>
       </c>
       <c r="F23" s="14" t="inlineStr">
@@ -1403,7 +1435,7 @@
       </c>
       <c r="E24" s="14" t="inlineStr">
         <is>
-          <t>600 TL</t>
+          <t>780 TL</t>
         </is>
       </c>
       <c r="F24" s="14" t="inlineStr">
@@ -1455,7 +1487,7 @@
       </c>
       <c r="E25" s="14" t="inlineStr">
         <is>
-          <t>600 TL</t>
+          <t>780 TL</t>
         </is>
       </c>
       <c r="F25" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-23 06:44:32 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -631,7 +631,11 @@
           <t>9 TL - 9 TL</t>
         </is>
       </c>
-      <c r="H2" s="14" t="inlineStr"/>
+      <c r="H2" s="14" t="inlineStr">
+        <is>
+          <t>15 TL - 15 TL</t>
+        </is>
+      </c>
       <c r="I2" s="14" t="inlineStr">
         <is>
           <t>18 TL - 18 TL</t>
@@ -666,11 +670,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -694,11 +694,7 @@
       </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -722,11 +718,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -748,7 +740,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -804,7 +800,11 @@
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
         </is>
       </c>
-      <c r="H7" s="14" t="inlineStr"/>
+      <c r="H7" s="14" t="inlineStr">
+        <is>
+          <t>%3,09</t>
+        </is>
+      </c>
       <c r="I7" s="14" t="inlineStr"/>
       <c r="J7" s="14" t="inlineStr">
         <is>
@@ -835,11 +835,7 @@
       </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -863,11 +859,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -891,11 +883,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -946,7 +934,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -974,17 +966,17 @@
           <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1018,17 +1010,17 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-24 06:41:09 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -670,7 +670,11 @@
       </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -694,7 +698,11 @@
       </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -718,7 +726,11 @@
       </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -740,11 +752,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -835,7 +843,11 @@
       </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -859,7 +871,11 @@
       </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -883,7 +899,11 @@
       </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -934,11 +954,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -963,20 +979,20 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1010,17 +1026,17 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-25 06:41:32 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -752,7 +752,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -954,7 +958,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -982,7 +990,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -1011,7 +1023,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1038,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-26 06:46:31 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -987,7 +987,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-27 06:43:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,11 +616,7 @@
           <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr">
-        <is>
-          <t>26 TL - 26 TL</t>
-        </is>
-      </c>
+      <c r="E2" s="14" t="inlineStr"/>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>28,57 TL - 28,57 TL</t>
@@ -663,18 +659,10 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -691,18 +679,10 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -719,18 +699,10 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -747,11 +719,7 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -840,18 +808,10 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -868,18 +828,10 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -896,18 +848,10 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -924,11 +868,7 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
@@ -953,11 +893,7 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -985,11 +921,7 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -1000,11 +932,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1033,11 +961,7 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>3.500 TL - 13.500 TL</t>
@@ -1048,11 +972,7 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-28 06:44:46 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,7 +616,11 @@
           <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr"/>
+      <c r="E2" s="14" t="inlineStr">
+        <is>
+          <t>26 TL - 26 TL</t>
+        </is>
+      </c>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>28,57 TL - 28,57 TL</t>
@@ -659,10 +663,18 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -679,10 +691,18 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -699,10 +719,18 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>30,46 TL - 60,94 TL - 609,43 TL</t>
@@ -719,12 +747,12 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -808,10 +836,18 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -828,10 +864,18 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -848,10 +892,18 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>15,23 TL - 30,47 TL - 211,05 TL</t>
@@ -868,7 +920,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
@@ -893,12 +949,12 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -921,18 +977,22 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -951,7 +1011,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
         </is>
       </c>
     </row>
@@ -961,18 +1021,22 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>6.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-29 06:56:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -677,7 +677,7 @@
       </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
         </is>
       </c>
       <c r="H3" s="14" t="inlineStr"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
         </is>
       </c>
       <c r="H4" s="14" t="inlineStr"/>
@@ -733,7 +733,7 @@
       </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
         </is>
       </c>
       <c r="H5" s="14" t="inlineStr"/>
@@ -752,7 +752,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -761,7 +765,7 @@
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+          <t>8.300,01 TL - 99,71 TL</t>
         </is>
       </c>
       <c r="H6" s="14" t="inlineStr">
@@ -850,7 +854,7 @@
       </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
         </is>
       </c>
       <c r="H8" s="14" t="inlineStr"/>
@@ -878,7 +882,7 @@
       </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
         </is>
       </c>
       <c r="H9" s="14" t="inlineStr"/>
@@ -906,7 +910,7 @@
       </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
-          <t>15,23 TL - 30,47 TL - 211,05 TL</t>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
         </is>
       </c>
       <c r="H10" s="14" t="inlineStr"/>
@@ -930,7 +934,7 @@
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
         </is>
       </c>
       <c r="H11" s="14" t="inlineStr"/>
@@ -954,7 +958,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -982,7 +990,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -1026,7 +1038,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
@@ -1039,7 +1055,7 @@
       </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
-          <t>6.300 TL - 6,09 TL</t>
+          <t>8.300 TL - 7,97 TL</t>
         </is>
       </c>
       <c r="H14" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-01-30 06:58:55 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -677,7 +677,7 @@
       </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
-          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
+          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
         </is>
       </c>
       <c r="H3" s="14" t="inlineStr"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
-          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
+          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
         </is>
       </c>
       <c r="H4" s="14" t="inlineStr"/>
@@ -733,7 +733,7 @@
       </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
-          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
+          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
         </is>
       </c>
       <c r="H5" s="14" t="inlineStr"/>
@@ -765,14 +765,10 @@
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
-          <t>8.300,01 TL - 99,71 TL</t>
-        </is>
-      </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+          <t>8.300,01 TL - 76,17 TL</t>
+        </is>
+      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -854,7 +850,7 @@
       </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
+          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
         </is>
       </c>
       <c r="H8" s="14" t="inlineStr"/>
@@ -882,7 +878,7 @@
       </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
-          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
+          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
         </is>
       </c>
       <c r="H9" s="14" t="inlineStr"/>
@@ -910,7 +906,7 @@
       </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
-          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
       <c r="H10" s="14" t="inlineStr"/>
@@ -934,7 +930,7 @@
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
-          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
+          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
         </is>
       </c>
       <c r="H11" s="14" t="inlineStr"/>
@@ -997,7 +993,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1006,11 +1002,7 @@
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
@@ -1055,14 +1047,10 @@
       </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
-          <t>8.300 TL - 7,97 TL</t>
-        </is>
-      </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>3.000 TL - 6.000 TL</t>
-        </is>
-      </c>
+          <t>8.300 TL - 6,09 TL</t>
+        </is>
+      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-01-31 06:47:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -670,11 +670,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -698,11 +694,7 @@
       </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -726,11 +718,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -768,7 +756,11 @@
           <t>8.300,01 TL - 76,17 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -843,11 +835,7 @@
       </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -871,11 +859,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -899,11 +883,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -993,16 +973,16 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
+      <c r="H13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
+        </is>
+      </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
@@ -1015,7 +995,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -1040,17 +1020,17 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 6,09 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>3.000 TL - 6.000 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-01 06:58:47 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -670,7 +670,11 @@
       </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -694,7 +698,11 @@
       </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -718,7 +726,11 @@
       </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -835,7 +847,11 @@
       </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -859,7 +875,11 @@
       </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -883,7 +903,11 @@
       </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -973,10 +997,14 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1020,7 +1048,11 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-02 07:10:45 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -752,11 +752,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -958,11 +954,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -990,14 +982,10 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -1038,11 +1026,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-03 07:00:33 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,11 +611,7 @@
           <t>30 TL - 30 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr">
-        <is>
-          <t>33,33 TL - 33,33 TL</t>
-        </is>
-      </c>
+      <c r="D2" s="14" t="inlineStr"/>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>26 TL - 26 TL</t>
@@ -643,7 +639,7 @@
       </c>
       <c r="J2" s="14" t="inlineStr">
         <is>
-          <t>25 TL - 25 TL</t>
+          <t>65 TL - 65 TL</t>
         </is>
       </c>
       <c r="K2" s="14" t="inlineStr">
@@ -792,11 +788,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr">
-        <is>
-          <t>%1,6</t>
-        </is>
-      </c>
+      <c r="D7" s="14" t="inlineStr"/>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-04 07:02:05 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,7 +611,11 @@
           <t>30 TL - 30 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr"/>
+      <c r="D2" s="14" t="inlineStr">
+        <is>
+          <t>33,33 TL - 33,33 TL</t>
+        </is>
+      </c>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>26 TL - 26 TL</t>
@@ -666,11 +670,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -694,11 +694,7 @@
       </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -722,11 +718,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -748,7 +740,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -788,7 +784,11 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr"/>
+      <c r="D7" s="14" t="inlineStr">
+        <is>
+          <t>%1,6</t>
+        </is>
+      </c>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -835,11 +835,7 @@
       </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -863,11 +859,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -891,11 +883,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -946,7 +934,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -971,20 +963,20 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1018,17 +1010,17 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-05 07:08:29 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -670,7 +670,11 @@
       </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr"/>
+      <c r="F3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -694,7 +698,11 @@
       </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr"/>
+      <c r="F4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -718,7 +726,11 @@
       </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr"/>
+      <c r="F5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -835,7 +847,11 @@
       </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr"/>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -859,7 +875,11 @@
       </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr"/>
+      <c r="F9" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -883,7 +903,11 @@
       </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
+        </is>
+      </c>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -963,7 +987,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -976,7 +1000,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1020,7 +1048,11 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>1.952,38 TL - 9.523,81 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 6,09 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-06 07:04:12 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -752,11 +752,7 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -773,11 +769,7 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -958,11 +950,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -990,11 +978,7 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -1011,11 +995,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
-        </is>
-      </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
@@ -1038,11 +1018,7 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-07 06:50:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -752,7 +752,11 @@
           <t>6,09 TL - 12,19 TL - 152,35 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -769,7 +773,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -950,7 +958,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -978,7 +990,11 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -995,10 +1011,14 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 9.335 TL</t>
         </is>
       </c>
       <c r="K13" s="14" t="inlineStr">
@@ -1018,7 +1038,11 @@
           <t>40.000 TL - 1.904,76 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-08 06:59:53 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -1018,7 +1018,7 @@
       </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 9.335 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
       <c r="K13" s="14" t="inlineStr">
@@ -1462,11 +1462,7 @@
           <t>780 TL</t>
         </is>
       </c>
-      <c r="F24" s="14" t="inlineStr">
-        <is>
-          <t>457,14 TL</t>
-        </is>
-      </c>
+      <c r="F24" s="14" t="inlineStr"/>
       <c r="G24" s="14" t="inlineStr">
         <is>
           <t>160 TL</t>
@@ -1514,11 +1510,7 @@
           <t>780 TL</t>
         </is>
       </c>
-      <c r="F25" s="14" t="inlineStr">
-        <is>
-          <t>380,95 TL</t>
-        </is>
-      </c>
+      <c r="F25" s="14" t="inlineStr"/>
       <c r="G25" s="14" t="inlineStr"/>
       <c r="H25" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-09 07:12:34 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -663,11 +663,7 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr">
@@ -691,11 +687,7 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr">
@@ -719,11 +711,7 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr">
@@ -747,16 +735,8 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
-        <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -778,11 +758,7 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="J6" s="14" t="inlineStr"/>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>7,97 TL - 15,96 TL - 199,41 TL</t>
@@ -840,11 +816,7 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr">
@@ -868,11 +840,7 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr">
@@ -896,11 +864,7 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr">
@@ -924,11 +888,7 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
@@ -953,16 +913,8 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -985,16 +937,8 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -1016,11 +960,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
+      <c r="J13" s="14" t="inlineStr"/>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1033,16 +973,8 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 1.904,76 TL</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
@@ -1064,11 +996,7 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.554,97 TL - 7.784 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>2.000 TL - 24.000 TL</t>
@@ -1462,7 +1390,11 @@
           <t>780 TL</t>
         </is>
       </c>
-      <c r="F24" s="14" t="inlineStr"/>
+      <c r="F24" s="14" t="inlineStr">
+        <is>
+          <t>457,14 TL</t>
+        </is>
+      </c>
       <c r="G24" s="14" t="inlineStr">
         <is>
           <t>160 TL</t>
@@ -1510,7 +1442,11 @@
           <t>780 TL</t>
         </is>
       </c>
-      <c r="F25" s="14" t="inlineStr"/>
+      <c r="F25" s="14" t="inlineStr">
+        <is>
+          <t>380,95 TL</t>
+        </is>
+      </c>
       <c r="G25" s="14" t="inlineStr"/>
       <c r="H25" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-10 07:13:12 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -623,7 +623,7 @@
       </c>
       <c r="F2" s="14" t="inlineStr">
         <is>
-          <t>28,57 TL - 28,57 TL</t>
+          <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
       <c r="G2" s="14" t="inlineStr">
@@ -663,14 +663,14 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr"/>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
-      <c r="F3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
           <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
@@ -687,14 +687,14 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
           <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
@@ -711,14 +711,14 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
+        </is>
+      </c>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
-      <c r="F5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
           <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
@@ -735,8 +735,16 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+        </is>
+      </c>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -816,14 +824,14 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr"/>
+      <c r="C8" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
           <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
@@ -840,14 +848,14 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr"/>
+      <c r="C9" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
-      <c r="F9" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
           <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
@@ -864,14 +872,14 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr"/>
+      <c r="C10" s="14" t="inlineStr">
+        <is>
+          <t>14,29 TL - 28,57 TL - 300 TL</t>
+        </is>
+      </c>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>15,23 TL - 30,47 TL - 304,71 TL</t>
-        </is>
-      </c>
+      <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
           <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
@@ -888,7 +896,11 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
+        </is>
+      </c>
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
@@ -913,8 +925,16 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -937,8 +957,16 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -946,7 +974,7 @@
       </c>
       <c r="F13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 300 TL | Azami 3.080 TL</t>
+          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr"/>
@@ -973,8 +1001,16 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 1.904,76 TL</t>
+        </is>
+      </c>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
@@ -982,7 +1018,7 @@
       </c>
       <c r="F14" s="14" t="inlineStr">
         <is>
-          <t>1.952,38 TL - 9.523,81 TL</t>
+          <t>2.785,72 TL - 12.380,95 TL</t>
         </is>
       </c>
       <c r="G14" s="14" t="inlineStr">
@@ -1031,7 +1067,7 @@
       </c>
       <c r="F15" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 276,19 TL Azami Tutar: 276,19 TL / 23.789,5 TL</t>
+          <t>%0,5 Asgari Tutar: 361,9 TL Azami Tutar: 361,9 TL / 361,9 TL</t>
         </is>
       </c>
       <c r="G15" s="14" t="inlineStr">
@@ -1099,7 +1135,7 @@
       </c>
       <c r="F17" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 328,57 TL Azami Tutar: 328,57 TL</t>
+          <t>%0,5 Asgari Tutar: 427,62 TL Azami Tutar: 427,62 TL</t>
         </is>
       </c>
       <c r="G17" s="14" t="inlineStr">
@@ -1183,7 +1219,7 @@
       </c>
       <c r="F20" s="14" t="inlineStr">
         <is>
-          <t>95,24 TL</t>
+          <t>123,81 TL</t>
         </is>
       </c>
       <c r="G20" s="14" t="inlineStr"/>
@@ -1283,7 +1319,7 @@
       </c>
       <c r="F22" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 328,57 TL Azami Tutar: 328,57 TL / 1.283,81 TL</t>
+          <t>%0,5 Asgari Tutar: 427,62 TL Azami Tutar: 427,62 TL / 1.669,52 TL</t>
         </is>
       </c>
       <c r="G22" s="14" t="inlineStr">
@@ -1392,7 +1428,7 @@
       </c>
       <c r="F24" s="14" t="inlineStr">
         <is>
-          <t>457,14 TL</t>
+          <t>600 TL</t>
         </is>
       </c>
       <c r="G24" s="14" t="inlineStr">
@@ -1444,7 +1480,7 @@
       </c>
       <c r="F25" s="14" t="inlineStr">
         <is>
-          <t>380,95 TL</t>
+          <t>600 TL</t>
         </is>
       </c>
       <c r="G25" s="14" t="inlineStr"/>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-11 07:09:57 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -628,7 +628,7 @@
       </c>
       <c r="G2" s="14" t="inlineStr">
         <is>
-          <t>9 TL - 9 TL</t>
+          <t>15 TL - 15 TL</t>
         </is>
       </c>
       <c r="H2" s="14" t="inlineStr">
@@ -673,7 +673,7 @@
       <c r="F3" s="14" t="inlineStr"/>
       <c r="G3" s="14" t="inlineStr">
         <is>
-          <t>30,46 TRY - 60,94 TRY - 609,43 TRY</t>
+          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
         </is>
       </c>
       <c r="H3" s="14" t="inlineStr"/>
@@ -697,7 +697,7 @@
       <c r="F4" s="14" t="inlineStr"/>
       <c r="G4" s="14" t="inlineStr">
         <is>
-          <t>21,27 TRY - 42,55 TRY - 304,71 TRY</t>
+          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
         </is>
       </c>
       <c r="H4" s="14" t="inlineStr"/>
@@ -721,7 +721,7 @@
       <c r="F5" s="14" t="inlineStr"/>
       <c r="G5" s="14" t="inlineStr">
         <is>
-          <t>6,09 TRY - 12,19 TRY - 152,35 TRY</t>
+          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
         </is>
       </c>
       <c r="H5" s="14" t="inlineStr"/>
@@ -753,7 +753,7 @@
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
-          <t>8.300,01 TL - 76,17 TL</t>
+          <t>8.300,01 TL - 99,71 TL</t>
         </is>
       </c>
       <c r="H6" s="14" t="inlineStr">
@@ -766,7 +766,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>7,97 TL - 15,96 TL - 199,41 TL</t>
@@ -834,7 +838,7 @@
       <c r="F8" s="14" t="inlineStr"/>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>15,23 TRY - 30,47 TRY - 304,71 TRY</t>
+          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
         </is>
       </c>
       <c r="H8" s="14" t="inlineStr"/>
@@ -858,7 +862,7 @@
       <c r="F9" s="14" t="inlineStr"/>
       <c r="G9" s="14" t="inlineStr">
         <is>
-          <t>10,63 TRY - 21,27 TRY - 152,35 TRY</t>
+          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
         </is>
       </c>
       <c r="H9" s="14" t="inlineStr"/>
@@ -882,7 +886,7 @@
       <c r="F10" s="14" t="inlineStr"/>
       <c r="G10" s="14" t="inlineStr">
         <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
         </is>
       </c>
       <c r="H10" s="14" t="inlineStr"/>
@@ -906,7 +910,7 @@
       <c r="F11" s="14" t="inlineStr"/>
       <c r="G11" s="14" t="inlineStr">
         <is>
-          <t>3,04 TRY - 6,09 TRY - 76,17 TRY</t>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
         </is>
       </c>
       <c r="H11" s="14" t="inlineStr"/>
@@ -988,7 +992,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
@@ -1023,7 +1031,7 @@
       </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
-          <t>8.300 TL - 6,09 TL</t>
+          <t>8.300 TL - 7,97 TL</t>
         </is>
       </c>
       <c r="H14" s="14" t="inlineStr">
@@ -1032,7 +1040,11 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.554,97 TL - 7.784 TL</t>
+        </is>
+      </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>2.000 TL - 24.000 TL</t>
@@ -1135,12 +1147,12 @@
       </c>
       <c r="F17" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 427,62 TL Azami Tutar: 427,62 TL</t>
+          <t>%0,5 Asgari Tutar: 361,9 TL Azami Tutar: 361,9 TL / 361,9 TL</t>
         </is>
       </c>
       <c r="G17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar: 110 TL Azami Tutar: 110 TL</t>
+          <t xml:space="preserve"> Asgari Tutar: 300 TL Azami Tutar: 300 TL</t>
         </is>
       </c>
       <c r="H17" s="14" t="inlineStr">
@@ -1267,12 +1279,12 @@
       </c>
       <c r="F21" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 419,05 TL Azami Tutar: 419,05 TL / 2.428,57 TL</t>
+          <t>%0,5 Asgari Tutar: 544,76 TL Azami Tutar: 544,76 TL / 3.157,14 TL</t>
         </is>
       </c>
       <c r="G21" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">%0,16 Asgari Tutar: 110 TL Azami Tutar: </t>
+          <t xml:space="preserve">%0,16 Asgari Tutar: 300 TL Azami Tutar: </t>
         </is>
       </c>
       <c r="H21" s="14" t="inlineStr">
@@ -1371,12 +1383,12 @@
       </c>
       <c r="F23" s="14" t="inlineStr">
         <is>
-          <t>66,67 TL</t>
+          <t>86,67 TL</t>
         </is>
       </c>
       <c r="G23" s="14" t="inlineStr">
         <is>
-          <t>200 TL</t>
+          <t>600 TL</t>
         </is>
       </c>
       <c r="H23" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-12 07:10:40 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,11 +626,7 @@
           <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr">
-        <is>
-          <t>15 TL - 15 TL</t>
-        </is>
-      </c>
+      <c r="G2" s="14" t="inlineStr"/>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -671,11 +667,7 @@
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="inlineStr"/>
       <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr"/>
@@ -695,11 +687,7 @@
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="inlineStr"/>
       <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr"/>
@@ -719,11 +707,7 @@
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
-        </is>
-      </c>
+      <c r="G5" s="14" t="inlineStr"/>
       <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr"/>
@@ -745,17 +729,9 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 99,71 TL</t>
-        </is>
-      </c>
+      <c r="G6" s="14" t="inlineStr"/>
       <c r="H6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -795,11 +771,7 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr">
-        <is>
-          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
-        </is>
-      </c>
+      <c r="G7" s="14" t="inlineStr"/>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -836,11 +808,7 @@
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
-        </is>
-      </c>
+      <c r="G8" s="14" t="inlineStr"/>
       <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr"/>
@@ -860,11 +828,7 @@
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
-        </is>
-      </c>
+      <c r="G9" s="14" t="inlineStr"/>
       <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr"/>
@@ -884,11 +848,7 @@
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
-        </is>
-      </c>
+      <c r="G10" s="14" t="inlineStr"/>
       <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr"/>
@@ -908,11 +868,7 @@
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
-        </is>
-      </c>
+      <c r="G11" s="14" t="inlineStr"/>
       <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr"/>
@@ -941,11 +897,7 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -971,11 +923,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
-        </is>
-      </c>
+      <c r="E13" s="14" t="inlineStr"/>
       <c r="F13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
@@ -1019,21 +967,13 @@
           <t>3.500 TL - 13.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr">
-        <is>
-          <t>2.170 TL - 2.170 TL</t>
-        </is>
-      </c>
+      <c r="E14" s="14" t="inlineStr"/>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>2.785,72 TL - 12.380,95 TL</t>
         </is>
       </c>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>8.300 TL - 7,97 TL</t>
-        </is>
-      </c>
+      <c r="G14" s="14" t="inlineStr"/>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>3.000 TL - 6.000 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-13 07:07:42 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -626,7 +626,11 @@
           <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr"/>
+      <c r="G2" s="14" t="inlineStr">
+        <is>
+          <t>15 TL - 15 TL</t>
+        </is>
+      </c>
       <c r="H2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -667,7 +671,11 @@
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr"/>
@@ -687,7 +695,11 @@
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr"/>
@@ -707,7 +719,11 @@
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
+        </is>
+      </c>
       <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr"/>
@@ -731,7 +747,11 @@
       </c>
       <c r="E6" s="14" t="inlineStr"/>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 99,71 TL</t>
+        </is>
+      </c>
       <c r="H6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -771,7 +791,11 @@
           <t>%3</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr"/>
+      <c r="G7" s="14" t="inlineStr">
+        <is>
+          <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
+        </is>
+      </c>
       <c r="H7" s="14" t="inlineStr">
         <is>
           <t>%3,09</t>
@@ -808,7 +832,11 @@
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
+        </is>
+      </c>
       <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr"/>
@@ -828,7 +856,11 @@
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
+        </is>
+      </c>
       <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr"/>
@@ -848,7 +880,11 @@
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
+        </is>
+      </c>
       <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr"/>
@@ -868,7 +904,11 @@
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
+        <is>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
+        </is>
+      </c>
       <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr"/>
@@ -897,7 +937,11 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -924,11 +968,7 @@
         </is>
       </c>
       <c r="E13" s="14" t="inlineStr"/>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -968,12 +1008,12 @@
         </is>
       </c>
       <c r="E14" s="14" t="inlineStr"/>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>2.785,72 TL - 12.380,95 TL</t>
-        </is>
-      </c>
-      <c r="G14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr"/>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>8.300 TL - 7,97 TL</t>
+        </is>
+      </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>3.000 TL - 6.000 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-14 06:53:19 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -745,7 +745,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr"/>
+      <c r="E6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="inlineStr"/>
       <c r="G6" s="14" t="inlineStr">
         <is>
@@ -947,7 +951,7 @@
       <c r="J12" s="14" t="inlineStr"/>
       <c r="K12" s="14" t="inlineStr">
         <is>
-          <t>WU: ,USD–; Diğer: 404,16 TL–3.403,42 TL</t>
+          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
         </is>
       </c>
     </row>
@@ -967,8 +971,16 @@
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
         </is>
       </c>
-      <c r="E13" s="14" t="inlineStr"/>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="E13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1007,8 +1019,16 @@
           <t>3.500 TL - 13.500 TL</t>
         </is>
       </c>
-      <c r="E14" s="14" t="inlineStr"/>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="E14" s="14" t="inlineStr">
+        <is>
+          <t>2.170 TL - 2.170 TL</t>
+        </is>
+      </c>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>2.785,72 TL - 12.380,95 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 7,97 TL</t>
@@ -1027,7 +1047,7 @@
       </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
-          <t>2.000 TL - 24.000 TL</t>
+          <t>1.196,51 TL - 5.583,74 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-15 07:01:23 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -976,11 +976,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -1024,11 +1020,7 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>2.785,72 TL - 12.380,95 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 7,97 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-16 07:11:15 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -771,11 +771,7 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -936,7 +932,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+          <t>Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -949,11 +945,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -973,10 +965,14 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr"/>
+          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
+        </is>
+      </c>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -993,11 +989,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1020,7 +1012,11 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>2.785,72 TL - 12.380,95 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 7,97 TL</t>
@@ -1037,11 +1033,7 @@
           <t>1.554,97 TL - 7.784 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>1.196,51 TL - 5.583,74 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-17 07:08:05 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,11 +621,7 @@
           <t>26 TL - 26 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr">
-        <is>
-          <t>33,33 TL - 33,33 TL</t>
-        </is>
-      </c>
+      <c r="F2" s="14" t="inlineStr"/>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -771,7 +767,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -786,11 +786,7 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>%3</t>
-        </is>
-      </c>
+      <c r="F7" s="14" t="inlineStr"/>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -932,7 +928,7 @@
       </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
-          <t>Diğer: 700 TL–4.000 TL</t>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
         </is>
       </c>
       <c r="E12" s="14" t="inlineStr"/>
@@ -945,7 +941,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -989,7 +989,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1033,7 +1037,11 @@
           <t>1.554,97 TL - 7.784 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>1.196,51 TL - 5.583,74 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-18 07:10:16 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -621,7 +621,11 @@
           <t>26 TL - 26 TL</t>
         </is>
       </c>
-      <c r="F2" s="14" t="inlineStr"/>
+      <c r="F2" s="14" t="inlineStr">
+        <is>
+          <t>33,33 TL - 33,33 TL</t>
+        </is>
+      </c>
       <c r="G2" s="14" t="inlineStr">
         <is>
           <t>15 TL - 15 TL</t>
@@ -762,16 +766,8 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="J6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -786,7 +782,11 @@
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr"/>
-      <c r="F7" s="14" t="inlineStr"/>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>%3</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
           <t>1 TRY (Kredi kartı ile ödemelerde ek olarak nakit avans faizi uygulanır.)</t>
@@ -941,11 +941,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -965,7 +961,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -984,16 +980,8 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="J13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -1032,16 +1020,8 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.554,97 TL - 7.784 TL</t>
-        </is>
-      </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>1.196,51 TL - 5.583,74 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-19 07:09:35 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,11 +611,7 @@
           <t>30 TL - 30 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr">
-        <is>
-          <t>33,33 TL - 33,33 TL</t>
-        </is>
-      </c>
+      <c r="D2" s="14" t="inlineStr"/>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>26 TL - 26 TL</t>
@@ -663,11 +659,7 @@
           <t>HESAPTAN EFT - Şube</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C3" s="14" t="inlineStr"/>
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
@@ -687,11 +679,7 @@
           <t>HESAPTAN EFT - ATM</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="inlineStr"/>
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
@@ -711,11 +699,7 @@
           <t>HESAPTAN EFT - Mobil</t>
         </is>
       </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>30,46 TL - 60,94 TL - 609,43 TL</t>
-        </is>
-      </c>
+      <c r="C5" s="14" t="inlineStr"/>
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
@@ -737,7 +721,7 @@
       </c>
       <c r="C6" s="14" t="inlineStr">
         <is>
-          <t>6,09 TL - 12,19 TL - 152,35 TL</t>
+          <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
@@ -766,8 +750,16 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -776,11 +768,7 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr">
-        <is>
-          <t>%1,6</t>
-        </is>
-      </c>
+      <c r="D7" s="14" t="inlineStr"/>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -820,11 +808,7 @@
           <t>HESAPTAN HAVALE - Şube</t>
         </is>
       </c>
-      <c r="C8" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="inlineStr"/>
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
@@ -844,11 +828,7 @@
           <t>HESAPTAN HAVALE - ATM</t>
         </is>
       </c>
-      <c r="C9" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C9" s="14" t="inlineStr"/>
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
@@ -868,11 +848,7 @@
           <t>HESAPTAN HAVALE - Mobil</t>
         </is>
       </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>14,29 TL - 28,57 TL - 300 TL</t>
-        </is>
-      </c>
+      <c r="C10" s="14" t="inlineStr"/>
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
@@ -892,11 +868,7 @@
           <t>DÜZENLİ HAVALE</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>3,04 TL - 6,09 TL - 76,17 TL</t>
-        </is>
-      </c>
+      <c r="C11" s="14" t="inlineStr"/>
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
@@ -941,7 +913,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -951,7 +927,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -980,8 +956,16 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -991,7 +975,7 @@
       </c>
       <c r="C14" s="14" t="inlineStr">
         <is>
-          <t>40.000 TL - 1.904,76 TL</t>
+          <t>40.000 TL - 2.485,72 TL</t>
         </is>
       </c>
       <c r="D14" s="14" t="inlineStr">
@@ -1020,8 +1004,16 @@
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.554,97 TL - 7.784 TL</t>
+        </is>
+      </c>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>1.196,51 TL - 5.583,74 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1036,7 +1028,7 @@
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar: 295,24 TL Azami Tutar: 295,24 TL</t>
+          <t xml:space="preserve"> Asgari Tutar: 390,48 TL Azami Tutar: 390,48 TL</t>
         </is>
       </c>
       <c r="D15" s="14" t="inlineStr">
@@ -1104,7 +1096,7 @@
       </c>
       <c r="C17" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Asgari Tutar: 200 TL Azami Tutar: 200 TL</t>
+          <t xml:space="preserve"> Asgari Tutar: 257,15 TL Azami Tutar: 257,15 TL</t>
         </is>
       </c>
       <c r="D17" s="14" t="inlineStr">
@@ -1188,7 +1180,7 @@
       </c>
       <c r="C20" s="14" t="inlineStr">
         <is>
-          <t>85,71 TL</t>
+          <t>114,29 TL</t>
         </is>
       </c>
       <c r="D20" s="14" t="inlineStr">
@@ -1236,7 +1228,7 @@
       </c>
       <c r="C21" s="14" t="inlineStr">
         <is>
-          <t>%0,57 Asgari Tutar: 447,62 TL Azami Tutar: 447,62 TL / 2.514,29 TL</t>
+          <t>%0,57 Asgari Tutar: 590,48 TL Azami Tutar: 590,48 TL / 3.295,24 TL</t>
         </is>
       </c>
       <c r="D21" s="14" t="inlineStr">
@@ -1340,7 +1332,7 @@
       </c>
       <c r="C23" s="14" t="inlineStr">
         <is>
-          <t>66,67 TL</t>
+          <t>85,72 TL</t>
         </is>
       </c>
       <c r="D23" s="14" t="inlineStr">
@@ -1397,7 +1389,7 @@
       </c>
       <c r="C24" s="14" t="inlineStr">
         <is>
-          <t>457,14 TL</t>
+          <t>600 TL</t>
         </is>
       </c>
       <c r="D24" s="14" t="inlineStr">
@@ -1449,7 +1441,7 @@
       </c>
       <c r="C25" s="14" t="inlineStr">
         <is>
-          <t>380,95 TL</t>
+          <t>495,24 TL</t>
         </is>
       </c>
       <c r="D25" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-20 07:05:36 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -611,7 +611,11 @@
           <t>30 TL - 30 TL</t>
         </is>
       </c>
-      <c r="D2" s="14" t="inlineStr"/>
+      <c r="D2" s="14" t="inlineStr">
+        <is>
+          <t>33,33 TL - 33,33 TL</t>
+        </is>
+      </c>
       <c r="E2" s="14" t="inlineStr">
         <is>
           <t>26 TL - 26 TL</t>
@@ -663,11 +667,7 @@
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="inlineStr"/>
       <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr"/>
@@ -683,11 +683,7 @@
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="inlineStr"/>
       <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr"/>
@@ -703,11 +699,7 @@
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
-        </is>
-      </c>
+      <c r="G5" s="14" t="inlineStr"/>
       <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr"/>
@@ -719,42 +711,30 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr">
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="E6" s="14" t="inlineStr">
+      <c r="F6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr"/>
+      <c r="H6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 99,71 TL</t>
-        </is>
-      </c>
-      <c r="H6" s="14" t="inlineStr">
+      <c r="I6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="J6" s="14" t="inlineStr"/>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>7,97 TL - 15,96 TL - 199,41 TL</t>
@@ -768,7 +748,11 @@
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr"/>
-      <c r="D7" s="14" t="inlineStr"/>
+      <c r="D7" s="14" t="inlineStr">
+        <is>
+          <t>%1,6</t>
+        </is>
+      </c>
       <c r="E7" s="14" t="inlineStr"/>
       <c r="F7" s="14" t="inlineStr">
         <is>
@@ -812,11 +796,7 @@
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
-        </is>
-      </c>
+      <c r="G8" s="14" t="inlineStr"/>
       <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr"/>
@@ -832,11 +812,7 @@
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
-        </is>
-      </c>
+      <c r="G9" s="14" t="inlineStr"/>
       <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr"/>
@@ -852,11 +828,7 @@
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
-        </is>
-      </c>
+      <c r="G10" s="14" t="inlineStr"/>
       <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr"/>
@@ -872,11 +844,7 @@
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
-        </is>
-      </c>
+      <c r="G11" s="14" t="inlineStr"/>
       <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr"/>
@@ -893,11 +861,7 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 1.000,01 USD–9,51 USD</t>
-        </is>
-      </c>
+      <c r="C12" s="14" t="inlineStr"/>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -905,11 +869,7 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
-        </is>
-      </c>
+      <c r="G12" s="14" t="inlineStr"/>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -925,11 +885,7 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
-        </is>
-      </c>
+      <c r="C13" s="14" t="inlineStr"/>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -956,14 +912,10 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
-        </is>
-      </c>
+      <c r="J13" s="14" t="inlineStr"/>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
         </is>
       </c>
     </row>
@@ -973,11 +925,7 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>40.000 TL - 2.485,72 TL</t>
-        </is>
-      </c>
+      <c r="C14" s="14" t="inlineStr"/>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>3.500 TL - 13.500 TL</t>
@@ -993,22 +941,14 @@
           <t>2.785,72 TL - 12.380,95 TL</t>
         </is>
       </c>
-      <c r="G14" s="14" t="inlineStr">
-        <is>
-          <t>8.300 TL - 7,97 TL</t>
-        </is>
-      </c>
+      <c r="G14" s="14" t="inlineStr"/>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>3.000 TL - 6.000 TL</t>
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr">
-        <is>
-          <t>1.554,97 TL - 7.784 TL</t>
-        </is>
-      </c>
+      <c r="J14" s="14" t="inlineStr"/>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>1.196,51 TL - 5.583,74 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-21 06:49:59 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -667,7 +667,11 @@
       <c r="D3" s="14" t="inlineStr"/>
       <c r="E3" s="14" t="inlineStr"/>
       <c r="F3" s="14" t="inlineStr"/>
-      <c r="G3" s="14" t="inlineStr"/>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>39,87 TRY - 79,76 TRY - 797,68 TRY</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="inlineStr"/>
       <c r="I3" s="14" t="inlineStr"/>
       <c r="J3" s="14" t="inlineStr"/>
@@ -683,7 +687,11 @@
       <c r="D4" s="14" t="inlineStr"/>
       <c r="E4" s="14" t="inlineStr"/>
       <c r="F4" s="14" t="inlineStr"/>
-      <c r="G4" s="14" t="inlineStr"/>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>27,84 TRY - 55,69 TRY - 398,83 TRY</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="inlineStr"/>
       <c r="I4" s="14" t="inlineStr"/>
       <c r="J4" s="14" t="inlineStr"/>
@@ -699,7 +707,11 @@
       <c r="D5" s="14" t="inlineStr"/>
       <c r="E5" s="14" t="inlineStr"/>
       <c r="F5" s="14" t="inlineStr"/>
-      <c r="G5" s="14" t="inlineStr"/>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TRY - 15,96 TRY - 199,41 TRY</t>
+        </is>
+      </c>
       <c r="H5" s="14" t="inlineStr"/>
       <c r="I5" s="14" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr"/>
@@ -711,7 +723,11 @@
           <t>DÜZENLİ EFT</t>
         </is>
       </c>
-      <c r="C6" s="14" t="inlineStr"/>
+      <c r="C6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -723,7 +739,11 @@
         </is>
       </c>
       <c r="F6" s="14" t="inlineStr"/>
-      <c r="G6" s="14" t="inlineStr"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 99,71 TL</t>
+        </is>
+      </c>
       <c r="H6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -734,7 +754,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="J6" s="14" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
           <t>7,97 TL - 15,96 TL - 199,41 TL</t>
@@ -796,7 +820,11 @@
       <c r="D8" s="14" t="inlineStr"/>
       <c r="E8" s="14" t="inlineStr"/>
       <c r="F8" s="14" t="inlineStr"/>
-      <c r="G8" s="14" t="inlineStr"/>
+      <c r="G8" s="14" t="inlineStr">
+        <is>
+          <t>19,94 TRY - 39,88 TRY - 398,84 TRY</t>
+        </is>
+      </c>
       <c r="H8" s="14" t="inlineStr"/>
       <c r="I8" s="14" t="inlineStr"/>
       <c r="J8" s="14" t="inlineStr"/>
@@ -812,7 +840,11 @@
       <c r="D9" s="14" t="inlineStr"/>
       <c r="E9" s="14" t="inlineStr"/>
       <c r="F9" s="14" t="inlineStr"/>
-      <c r="G9" s="14" t="inlineStr"/>
+      <c r="G9" s="14" t="inlineStr">
+        <is>
+          <t>13,92 TRY - 27,85 TRY - 199,42 TRY</t>
+        </is>
+      </c>
       <c r="H9" s="14" t="inlineStr"/>
       <c r="I9" s="14" t="inlineStr"/>
       <c r="J9" s="14" t="inlineStr"/>
@@ -828,7 +860,11 @@
       <c r="D10" s="14" t="inlineStr"/>
       <c r="E10" s="14" t="inlineStr"/>
       <c r="F10" s="14" t="inlineStr"/>
-      <c r="G10" s="14" t="inlineStr"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
+        </is>
+      </c>
       <c r="H10" s="14" t="inlineStr"/>
       <c r="I10" s="14" t="inlineStr"/>
       <c r="J10" s="14" t="inlineStr"/>
@@ -844,7 +880,11 @@
       <c r="D11" s="14" t="inlineStr"/>
       <c r="E11" s="14" t="inlineStr"/>
       <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
+      <c r="G11" s="14" t="inlineStr">
+        <is>
+          <t>3,99 TRY - 7,98 TRY - 99,71 TRY</t>
+        </is>
+      </c>
       <c r="H11" s="14" t="inlineStr"/>
       <c r="I11" s="14" t="inlineStr"/>
       <c r="J11" s="14" t="inlineStr"/>
@@ -861,7 +901,11 @@
           <t>GİDEN SWIFT</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
+      <c r="C12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 1.000,01 USD–9,51 USD</t>
+        </is>
+      </c>
       <c r="D12" s="14" t="inlineStr">
         <is>
           <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
@@ -869,7 +913,11 @@
       </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
+      <c r="G12" s="14" t="inlineStr">
+        <is>
+          <t>Şube (Kasadan): %0,5; Şube (Hesaptan): %0,75; İnternet: 15 USD</t>
+        </is>
+      </c>
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
@@ -885,7 +933,11 @@
           <t>GELEN SWIFT</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr"/>
+      <c r="C13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
@@ -896,11 +948,7 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -912,10 +960,14 @@
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="J13" s="14" t="inlineStr"/>
+      <c r="J13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
+        </is>
+      </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -925,7 +977,11 @@
           <t>GİDEN SWIFT - Mobil</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr"/>
+      <c r="C14" s="14" t="inlineStr">
+        <is>
+          <t>40.000 TL - 2.485,72 TL</t>
+        </is>
+      </c>
       <c r="D14" s="14" t="inlineStr">
         <is>
           <t>3.500 TL - 13.500 TL</t>
@@ -936,19 +992,23 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>2.785,72 TL - 12.380,95 TL</t>
-        </is>
-      </c>
-      <c r="G14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr"/>
+      <c r="G14" s="14" t="inlineStr">
+        <is>
+          <t>8.300 TL - 7,97 TL</t>
+        </is>
+      </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
           <t>3.000 TL - 6.000 TL</t>
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr"/>
-      <c r="J14" s="14" t="inlineStr"/>
+      <c r="J14" s="14" t="inlineStr">
+        <is>
+          <t>1.554,97 TL - 7.784 TL</t>
+        </is>
+      </c>
       <c r="K14" s="14" t="inlineStr">
         <is>
           <t>1.196,51 TL - 5.583,74 TL</t>
@@ -1003,7 +1063,7 @@
       </c>
       <c r="J15" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 250 TL Azami Tutar: 250 TL / 4.000 TL</t>
+          <t>%0,5 Asgari Tutar: 375 TL Azami Tutar: 375 TL / 6.500 TL</t>
         </is>
       </c>
       <c r="K15" s="14" t="inlineStr">
@@ -1071,7 +1131,7 @@
       </c>
       <c r="J17" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 250 TL Azami Tutar: 250 TL / 3.500 TL</t>
+          <t>%0,5 Asgari Tutar: 350 TL Azami Tutar: 350 TL / 5.500 TL</t>
         </is>
       </c>
       <c r="K17" s="14" t="inlineStr">
@@ -1151,7 +1211,7 @@
       </c>
       <c r="J20" s="14" t="inlineStr">
         <is>
-          <t>100 TL</t>
+          <t>200 TL</t>
         </is>
       </c>
       <c r="K20" s="14" t="inlineStr">
@@ -1203,7 +1263,7 @@
       </c>
       <c r="J21" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 350 TL Azami Tutar: 350 TL / 2.500 TL</t>
+          <t>%0,5 Asgari Tutar: 500 TL Azami Tutar: 500 TL / 5.000 TL</t>
         </is>
       </c>
       <c r="K21" s="14" t="inlineStr">
@@ -1255,7 +1315,7 @@
       </c>
       <c r="J22" s="14" t="inlineStr">
         <is>
-          <t>%0,5 Asgari Tutar: 750 TL Azami Tutar: 750 TL / 5.500 TL</t>
+          <t>%0,5 Asgari Tutar: 1.500 TL Azami Tutar: 1.500 TL / 9.000 TL</t>
         </is>
       </c>
       <c r="K22" s="14" t="inlineStr">
@@ -1307,7 +1367,7 @@
       </c>
       <c r="J23" s="14" t="inlineStr">
         <is>
-          <t>50 TL</t>
+          <t>75 TL</t>
         </is>
       </c>
       <c r="K23" s="14" t="inlineStr">
@@ -1364,7 +1424,7 @@
       </c>
       <c r="J24" s="14" t="inlineStr">
         <is>
-          <t>375 TL</t>
+          <t>500 TL</t>
         </is>
       </c>
       <c r="K24" s="14" t="inlineStr">
@@ -1412,7 +1472,7 @@
       </c>
       <c r="J25" s="14" t="inlineStr">
         <is>
-          <t>375 TL</t>
+          <t>750 TL</t>
         </is>
       </c>
       <c r="K25" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-22 06:57:28 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -948,7 +948,11 @@
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
@@ -992,7 +996,11 @@
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>2.785,72 TL - 12.380,95 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 7,97 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-23 07:13:27 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -945,7 +945,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-24 07:12:58 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,11 +616,7 @@
           <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr">
-        <is>
-          <t>26 TL - 26 TL</t>
-        </is>
-      </c>
+      <c r="E2" s="14" t="inlineStr"/>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>33,33 TL - 33,33 TL</t>
@@ -935,7 +931,7 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
         </is>
       </c>
       <c r="D13" s="14" t="inlineStr">
@@ -945,7 +941,7 @@
       </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 11.380 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
       <c r="F13" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-25 07:11:04 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -616,7 +616,11 @@
           <t>33,33 TL - 33,33 TL</t>
         </is>
       </c>
-      <c r="E2" s="14" t="inlineStr"/>
+      <c r="E2" s="14" t="inlineStr">
+        <is>
+          <t>26 TL - 26 TL</t>
+        </is>
+      </c>
       <c r="F2" s="14" t="inlineStr">
         <is>
           <t>33,33 TL - 33,33 TL</t>
@@ -724,11 +728,7 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -902,11 +902,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -931,14 +927,10 @@
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 0 TL | Azami 9.999.999.999.999 TL</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+          <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
+        </is>
+      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -967,7 +959,7 @@
       </c>
       <c r="K13" s="14" t="inlineStr">
         <is>
-          <t>Hesaba: Asgari 1 TL | Azami 69,62 TL</t>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
         </is>
       </c>
     </row>
@@ -982,11 +974,7 @@
           <t>40.000 TL - 2.485,72 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-26 07:09:54 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -728,7 +728,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -740,11 +744,7 @@
           <t>8.300,01 TL - 99,71 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="H6" s="14" t="inlineStr"/>
       <c r="I6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -902,7 +902,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -930,23 +934,19 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
-        </is>
-      </c>
+      <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
-        </is>
-      </c>
+      <c r="H13" s="14" t="inlineStr"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
@@ -974,27 +974,23 @@
           <t>40.000 TL - 2.485,72 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>2.785,72 TL - 12.380,95 TL</t>
-        </is>
-      </c>
+      <c r="F14" s="14" t="inlineStr"/>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 7,97 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr">
-        <is>
-          <t>3.000 TL - 6.000 TL</t>
-        </is>
-      </c>
+      <c r="H14" s="14" t="inlineStr"/>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update benchmark: 2026-02-27 07:04:35 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -728,11 +728,7 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr">
-        <is>
-          <t>8.300,01 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="inlineStr"/>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -744,22 +740,18 @@
           <t>8.300,01 TL - 99,71 TL</t>
         </is>
       </c>
-      <c r="H6" s="14" t="inlineStr"/>
-      <c r="I6" s="14" t="inlineStr">
+      <c r="H6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
+      <c r="I6" s="14" t="inlineStr"/>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr">
-        <is>
-          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
-        </is>
-      </c>
+      <c r="K6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -902,11 +894,7 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
-        </is>
-      </c>
+      <c r="D12" s="14" t="inlineStr"/>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -917,11 +905,7 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr">
-        <is>
-          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
-        </is>
-      </c>
+      <c r="K12" s="14" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -934,11 +918,7 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
-        </is>
-      </c>
+      <c r="D13" s="14" t="inlineStr"/>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
@@ -946,22 +926,18 @@
       </c>
       <c r="F13" s="14" t="inlineStr"/>
       <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="14" t="inlineStr"/>
-      <c r="I13" s="14" t="inlineStr">
+      <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
+      <c r="I13" s="14" t="inlineStr"/>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
-        </is>
-      </c>
+      <c r="K13" s="14" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -974,11 +950,7 @@
           <t>40.000 TL - 2.485,72 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr">
-        <is>
-          <t>3.500 TL - 13.500 TL</t>
-        </is>
-      </c>
+      <c r="D14" s="14" t="inlineStr"/>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
@@ -990,18 +962,18 @@
           <t>8.300 TL - 7,97 TL</t>
         </is>
       </c>
-      <c r="H14" s="14" t="inlineStr"/>
+      <c r="H14" s="14" t="inlineStr">
+        <is>
+          <t>3.000 TL - 6.000 TL</t>
+        </is>
+      </c>
       <c r="I14" s="14" t="inlineStr"/>
       <c r="J14" s="14" t="inlineStr">
         <is>
           <t>1.554,97 TL - 7.784 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>1.196,51 TL - 5.583,74 TL</t>
-        </is>
-      </c>
+      <c r="K14" s="14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">

</xml_diff>

<commit_message>
Update benchmark: 2026-02-28 06:47:11 UTC
</commit_message>
<xml_diff>
--- a/docs/Benchmark_Results.xlsx
+++ b/docs/Benchmark_Results.xlsx
@@ -728,7 +728,11 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="D6" s="14" t="inlineStr"/>
+      <c r="D6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
@@ -745,13 +749,21 @@
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="I6" s="14" t="inlineStr"/>
+      <c r="I6" s="14" t="inlineStr">
+        <is>
+          <t>8.300,01 TL - 199,41 TL</t>
+        </is>
+      </c>
       <c r="J6" s="14" t="inlineStr">
         <is>
           <t>8.300,01 TL - 199,41 TL</t>
         </is>
       </c>
-      <c r="K6" s="14" t="inlineStr"/>
+      <c r="K6" s="14" t="inlineStr">
+        <is>
+          <t>7,97 TL - 15,96 TL - 199,41 TL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="13" t="inlineStr">
@@ -894,7 +906,11 @@
           <t>WU: 1.000,01 USD–9,51 USD</t>
         </is>
       </c>
-      <c r="D12" s="14" t="inlineStr"/>
+      <c r="D12" s="14" t="inlineStr">
+        <is>
+          <t>WU: 0,75 USD–12 USD; Diğer: 700 TL–4.000 TL</t>
+        </is>
+      </c>
       <c r="E12" s="14" t="inlineStr"/>
       <c r="F12" s="14" t="inlineStr"/>
       <c r="G12" s="14" t="inlineStr">
@@ -905,7 +921,11 @@
       <c r="H12" s="14" t="inlineStr"/>
       <c r="I12" s="14" t="inlineStr"/>
       <c r="J12" s="14" t="inlineStr"/>
-      <c r="K12" s="14" t="inlineStr"/>
+      <c r="K12" s="14" t="inlineStr">
+        <is>
+          <t>WU: ,USD–; Diğer: 529 TL–4.454,74 TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="inlineStr">
@@ -918,26 +938,42 @@
           <t>Hesaba: Asgari 0 TL | Azami 0,94 TL</t>
         </is>
       </c>
-      <c r="D13" s="14" t="inlineStr"/>
+      <c r="D13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 909,5 TL</t>
+        </is>
+      </c>
       <c r="E13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 1.114 TL</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 795 TL | Azami 4.005 TL</t>
+        </is>
+      </c>
       <c r="G13" s="14" t="inlineStr"/>
       <c r="H13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
         </is>
       </c>
-      <c r="I13" s="14" t="inlineStr"/>
+      <c r="I13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 7,97 TL</t>
+        </is>
+      </c>
       <c r="J13" s="14" t="inlineStr">
         <is>
           <t>Hesaba: Asgari 1 TL | Azami 995,5 TL</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr"/>
+      <c r="K13" s="14" t="inlineStr">
+        <is>
+          <t>Hesaba: Asgari 1 TL | Azami 865,75 TL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="inlineStr">
@@ -950,13 +986,21 @@
           <t>40.000 TL - 2.485,72 TL</t>
         </is>
       </c>
-      <c r="D14" s="14" t="inlineStr"/>
+      <c r="D14" s="14" t="inlineStr">
+        <is>
+          <t>3.500 TL - 13.500 TL</t>
+        </is>
+      </c>
       <c r="E14" s="14" t="inlineStr">
         <is>
           <t>2.170 TL - 2.170 TL</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>2.785,72 TL - 12.380,95 TL</t>
+        </is>
+      </c>
       <c r="G14" s="14" t="inlineStr">
         <is>
           <t>8.300 TL - 7,97 TL</t>
@@ -973,7 +1017,11 @@
           <t>1.554,97 TL - 7.784 TL</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr"/>
+      <c r="K14" s="14" t="inlineStr">
+        <is>
+          <t>1.196,51 TL - 5.583,74 TL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1352,11 +1400,7 @@
           <t>600 TL</t>
         </is>
       </c>
-      <c r="D24" s="14" t="inlineStr">
-        <is>
-          <t>476,2 TL</t>
-        </is>
-      </c>
+      <c r="D24" s="14" t="inlineStr"/>
       <c r="E24" s="14" t="inlineStr">
         <is>
           <t>780 TL</t>
@@ -1404,11 +1448,7 @@
           <t>495,24 TL</t>
         </is>
       </c>
-      <c r="D25" s="14" t="inlineStr">
-        <is>
-          <t>428,58 TL</t>
-        </is>
-      </c>
+      <c r="D25" s="14" t="inlineStr"/>
       <c r="E25" s="14" t="inlineStr">
         <is>
           <t>780 TL</t>

</xml_diff>